<commit_message>
Delivery Note Negative Test cases
</commit_message>
<xml_diff>
--- a/tests/artifact/script/GNUKhata.macro.xlsx
+++ b/tests/artifact/script/GNUKhata.macro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9024" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -2483,12 +2483,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -2540,21 +2540,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -2563,18 +2548,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2587,6 +2588,37 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2594,15 +2626,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2616,55 +2649,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2679,6 +2665,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2705,7 +2705,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2717,7 +2717,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2729,7 +2735,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2741,19 +2843,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2765,127 +2885,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2915,16 +2915,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2944,37 +2962,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3005,16 +3003,24 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3023,139 +3029,133 @@
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3223,7 +3223,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3250,52 +3250,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -6290,7 +6290,7 @@
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="$A24:$XFD24"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
@@ -6880,7 +6880,7 @@
         <v>30</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>559</v>
+        <v>253</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>780</v>

</xml_diff>

<commit_message>
Mobile Tests of Unit Of Measurement page
</commit_message>
<xml_diff>
--- a/tests/artifact/script/GNUKhata.macro.xlsx
+++ b/tests/artifact/script/GNUKhata.macro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="784">
   <si>
     <t>target</t>
   </si>
@@ -2479,16 +2479,25 @@
   <si>
     <t>${title.header}</t>
   </si>
+  <si>
+    <t>Welcome Accion!</t>
+  </si>
+  <si>
+    <t>mobileLogin</t>
+  </si>
+  <si>
+    <t>Resize the window to mobile view</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -2525,12 +2534,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -2538,21 +2545,6 @@
       <color theme="0" tint="-0.0499893185216834"/>
       <name val="Tahoma"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -2563,18 +2555,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2587,6 +2595,37 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2594,15 +2633,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2616,55 +2656,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2679,6 +2672,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2705,7 +2712,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2717,7 +2724,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2729,7 +2742,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2741,19 +2850,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2765,127 +2892,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2915,16 +2922,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2944,37 +2969,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3005,161 +3010,163 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3215,17 +3222,8 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3250,52 +3248,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -6288,9 +6286,9 @@
   <dimension ref="A1:O192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="$A24:$XFD24"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
@@ -6337,10 +6335,10 @@
       <c r="I1" s="10" t="s">
         <v>731</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="19" t="s">
         <v>732</v>
       </c>
-      <c r="K1" s="22"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="10" t="s">
         <v>733</v>
       </c>
@@ -6368,8 +6366,8 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A3" s="11"/>
@@ -6390,8 +6388,8 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
     </row>
     <row r="4" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A4" s="11"/>
@@ -6414,8 +6412,8 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A5" s="11"/>
@@ -6436,8 +6434,8 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="22"/>
     </row>
     <row r="6" s="2" customFormat="1" ht="41.4" spans="1:12">
       <c r="A6" s="11" t="s">
@@ -6462,8 +6460,8 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="18" customHeight="1" spans="3:12">
       <c r="C7" s="13" t="s">
@@ -6482,8 +6480,8 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="22"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A8" s="11"/>
@@ -6504,8 +6502,8 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="22"/>
     </row>
     <row r="9" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A9" s="11"/>
@@ -6528,8 +6526,8 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="22"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A10" s="11"/>
@@ -6550,8 +6548,8 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" s="2" customFormat="1" ht="96.6" spans="1:12">
       <c r="A11" s="11" t="s">
@@ -6576,8 +6574,8 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="22"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A12" s="11"/>
@@ -6598,8 +6596,8 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A13" s="11"/>
@@ -6620,8 +6618,8 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="15"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="22"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A14" s="11"/>
@@ -6644,8 +6642,8 @@
       <c r="J14" s="15" t="s">
         <v>760</v>
       </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A15" s="11"/>
@@ -6664,8 +6662,8 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="22"/>
     </row>
     <row r="16" s="2" customFormat="1" ht="27.6" spans="1:15">
       <c r="A16" s="11" t="s">
@@ -6690,11 +6688,11 @@
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="23"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="21"/>
     </row>
     <row r="17" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="11"/>
@@ -6711,11 +6709,11 @@
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="23"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="21"/>
     </row>
     <row r="18" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="11"/>
@@ -6736,11 +6734,11 @@
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="23"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="21"/>
     </row>
     <row r="19" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="11"/>
@@ -6761,11 +6759,11 @@
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="23"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="21"/>
     </row>
     <row r="20" s="2" customFormat="1" ht="22" customHeight="1" spans="1:15">
       <c r="A20" s="11"/>
@@ -6786,11 +6784,11 @@
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="15"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="23"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="21"/>
     </row>
     <row r="21" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A21" s="11"/>
@@ -6813,11 +6811,11 @@
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="15"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="23"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="21"/>
     </row>
     <row r="22" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="11"/>
@@ -6840,11 +6838,11 @@
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="15"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="23"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="21"/>
     </row>
     <row r="23" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="11"/>
@@ -6865,13 +6863,13 @@
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="23"/>
-    </row>
-    <row r="24" s="2" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="K23" s="21"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="21"/>
+    </row>
+    <row r="24" s="2" customFormat="1" ht="30" customHeight="1" spans="1:15">
       <c r="A24" s="11"/>
       <c r="B24" s="12" t="s">
         <v>779</v>
@@ -6880,147 +6878,233 @@
         <v>30</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>559</v>
+        <v>530</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>780</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="18" t="s">
+        <v>781</v>
+      </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="23"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="21"/>
     </row>
     <row r="25" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="A25" s="11" t="s">
+        <v>782</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>763</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>764</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>765</v>
+      </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="22"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="B26" s="12" t="s">
+        <v>783</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="E26" s="14">
+        <v>430</v>
+      </c>
+      <c r="F26" s="14">
+        <v>932</v>
+      </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="24"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="22"/>
     </row>
     <row r="27" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="C27" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>767</v>
+      </c>
+      <c r="F27" s="17">
+        <v>5000</v>
+      </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="15"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="24"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="22"/>
     </row>
     <row r="28" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="B28" s="12" t="s">
+        <v>768</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>767</v>
+      </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="15"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="24"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="22"/>
     </row>
     <row r="29" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="B29" s="12" t="s">
+        <v>769</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>713</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>770</v>
+      </c>
+      <c r="F29" s="15"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="24"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="22"/>
     </row>
     <row r="30" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="B30" s="12" t="s">
+        <v>771</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>772</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>773</v>
+      </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="15"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="24"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="22"/>
     </row>
     <row r="31" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="14"/>
+      <c r="B31" s="12" t="s">
+        <v>774</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>775</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>776</v>
+      </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="15"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="24"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="22"/>
     </row>
     <row r="32" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="B32" s="12" t="s">
+        <v>777</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>778</v>
+      </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="15"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="24"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="22"/>
     </row>
     <row r="33" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="B33" s="12" t="s">
+        <v>779</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>780</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>781</v>
+      </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="15"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="24"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="22"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A34" s="11"/>
@@ -7033,8 +7117,8 @@
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="15"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="24"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="22"/>
     </row>
     <row r="35" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A35" s="11"/>
@@ -7047,8 +7131,8 @@
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="15"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="24"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="22"/>
     </row>
     <row r="36" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A36" s="11"/>
@@ -7061,8 +7145,8 @@
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="15"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="24"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="22"/>
     </row>
     <row r="37" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A37" s="11"/>
@@ -7075,8 +7159,8 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="15"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="24"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="22"/>
     </row>
     <row r="38" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A38" s="11"/>
@@ -7089,8 +7173,8 @@
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="24"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="22"/>
     </row>
     <row r="39" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A39" s="11"/>
@@ -7103,8 +7187,8 @@
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="15"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="24"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="22"/>
     </row>
     <row r="40" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A40" s="11"/>
@@ -7117,8 +7201,8 @@
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="15"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="24"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="22"/>
     </row>
     <row r="41" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A41" s="11"/>
@@ -7131,8 +7215,8 @@
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="15"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="24"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="22"/>
     </row>
     <row r="42" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A42" s="11"/>
@@ -7145,8 +7229,8 @@
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="24"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="22"/>
     </row>
     <row r="43" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A43" s="11"/>
@@ -7159,8 +7243,8 @@
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="15"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="24"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="22"/>
     </row>
     <row r="44" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A44" s="11"/>
@@ -7173,8 +7257,8 @@
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="15"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="24"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="22"/>
     </row>
     <row r="45" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A45" s="11"/>
@@ -7187,8 +7271,8 @@
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="15"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="24"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="22"/>
     </row>
     <row r="46" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A46" s="11"/>
@@ -7201,8 +7285,8 @@
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="15"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="24"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="22"/>
     </row>
     <row r="47" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A47" s="11"/>
@@ -7215,8 +7299,8 @@
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="15"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="24"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="22"/>
     </row>
     <row r="48" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A48" s="11"/>
@@ -7229,8 +7313,8 @@
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="15"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="24"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="22"/>
     </row>
     <row r="49" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A49" s="11"/>
@@ -7243,8 +7327,8 @@
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="24"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="22"/>
     </row>
     <row r="50" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A50" s="11"/>
@@ -7257,8 +7341,8 @@
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
       <c r="J50" s="15"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="24"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="22"/>
     </row>
     <row r="51" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A51" s="11"/>
@@ -7271,8 +7355,8 @@
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
       <c r="J51" s="15"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="24"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="22"/>
     </row>
     <row r="52" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A52" s="11"/>
@@ -7285,8 +7369,8 @@
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
       <c r="J52" s="15"/>
-      <c r="K52" s="23"/>
-      <c r="L52" s="24"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="22"/>
     </row>
     <row r="53" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A53" s="11"/>
@@ -7299,8 +7383,8 @@
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
       <c r="J53" s="15"/>
-      <c r="K53" s="23"/>
-      <c r="L53" s="24"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="22"/>
     </row>
     <row r="54" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A54" s="11"/>
@@ -7313,8 +7397,8 @@
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
       <c r="J54" s="15"/>
-      <c r="K54" s="23"/>
-      <c r="L54" s="24"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="22"/>
     </row>
     <row r="55" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A55" s="11"/>
@@ -7327,8 +7411,8 @@
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
       <c r="J55" s="15"/>
-      <c r="K55" s="23"/>
-      <c r="L55" s="24"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="22"/>
     </row>
     <row r="56" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A56" s="11"/>
@@ -7341,8 +7425,8 @@
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
       <c r="J56" s="15"/>
-      <c r="K56" s="23"/>
-      <c r="L56" s="24"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="22"/>
     </row>
     <row r="57" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A57" s="11"/>
@@ -7355,8 +7439,8 @@
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
       <c r="J57" s="15"/>
-      <c r="K57" s="23"/>
-      <c r="L57" s="24"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="22"/>
     </row>
     <row r="58" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A58" s="11"/>
@@ -7369,8 +7453,8 @@
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
       <c r="J58" s="15"/>
-      <c r="K58" s="23"/>
-      <c r="L58" s="24"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="22"/>
     </row>
     <row r="59" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A59" s="11"/>
@@ -7383,8 +7467,8 @@
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
       <c r="J59" s="15"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="24"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="22"/>
     </row>
     <row r="60" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A60" s="11"/>
@@ -7397,8 +7481,8 @@
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
       <c r="J60" s="15"/>
-      <c r="K60" s="23"/>
-      <c r="L60" s="24"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="22"/>
     </row>
     <row r="61" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A61" s="11"/>
@@ -7411,8 +7495,8 @@
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
       <c r="J61" s="15"/>
-      <c r="K61" s="23"/>
-      <c r="L61" s="24"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="22"/>
     </row>
     <row r="62" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A62" s="11"/>
@@ -7425,8 +7509,8 @@
       <c r="H62" s="14"/>
       <c r="I62" s="14"/>
       <c r="J62" s="15"/>
-      <c r="K62" s="23"/>
-      <c r="L62" s="24"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="22"/>
     </row>
     <row r="63" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A63" s="11"/>
@@ -7439,8 +7523,8 @@
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
       <c r="J63" s="15"/>
-      <c r="K63" s="23"/>
-      <c r="L63" s="24"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="22"/>
     </row>
     <row r="64" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A64" s="11"/>
@@ -7453,8 +7537,8 @@
       <c r="H64" s="14"/>
       <c r="I64" s="14"/>
       <c r="J64" s="15"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="24"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="22"/>
     </row>
     <row r="65" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A65" s="11"/>
@@ -7467,8 +7551,8 @@
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
       <c r="J65" s="15"/>
-      <c r="K65" s="23"/>
-      <c r="L65" s="24"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="22"/>
     </row>
     <row r="66" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A66" s="11"/>
@@ -7481,8 +7565,8 @@
       <c r="H66" s="14"/>
       <c r="I66" s="14"/>
       <c r="J66" s="15"/>
-      <c r="K66" s="23"/>
-      <c r="L66" s="24"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="22"/>
     </row>
     <row r="67" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A67" s="11"/>
@@ -7495,8 +7579,8 @@
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
       <c r="J67" s="15"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="24"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="22"/>
     </row>
     <row r="68" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A68" s="11"/>
@@ -7509,8 +7593,8 @@
       <c r="H68" s="14"/>
       <c r="I68" s="14"/>
       <c r="J68" s="15"/>
-      <c r="K68" s="23"/>
-      <c r="L68" s="24"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="22"/>
     </row>
     <row r="69" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A69" s="11"/>
@@ -7523,8 +7607,8 @@
       <c r="H69" s="14"/>
       <c r="I69" s="14"/>
       <c r="J69" s="15"/>
-      <c r="K69" s="23"/>
-      <c r="L69" s="24"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="22"/>
     </row>
     <row r="70" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A70" s="11"/>
@@ -7537,8 +7621,8 @@
       <c r="H70" s="14"/>
       <c r="I70" s="14"/>
       <c r="J70" s="15"/>
-      <c r="K70" s="23"/>
-      <c r="L70" s="24"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="22"/>
     </row>
     <row r="71" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A71" s="11"/>
@@ -7551,8 +7635,8 @@
       <c r="H71" s="14"/>
       <c r="I71" s="14"/>
       <c r="J71" s="15"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="24"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="22"/>
     </row>
     <row r="72" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A72" s="11"/>
@@ -7565,8 +7649,8 @@
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
       <c r="J72" s="15"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="24"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="22"/>
     </row>
     <row r="73" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A73" s="11"/>
@@ -7579,8 +7663,8 @@
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
       <c r="J73" s="15"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="24"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="22"/>
     </row>
     <row r="74" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A74" s="11"/>
@@ -7593,8 +7677,8 @@
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
       <c r="J74" s="15"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="24"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="22"/>
     </row>
     <row r="75" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A75" s="11"/>
@@ -7607,8 +7691,8 @@
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
       <c r="J75" s="15"/>
-      <c r="K75" s="23"/>
-      <c r="L75" s="24"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="22"/>
     </row>
     <row r="76" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A76" s="11"/>
@@ -7621,8 +7705,8 @@
       <c r="H76" s="14"/>
       <c r="I76" s="14"/>
       <c r="J76" s="15"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="24"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="22"/>
     </row>
     <row r="77" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A77" s="11"/>
@@ -7635,8 +7719,8 @@
       <c r="H77" s="14"/>
       <c r="I77" s="14"/>
       <c r="J77" s="15"/>
-      <c r="K77" s="23"/>
-      <c r="L77" s="24"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="22"/>
     </row>
     <row r="78" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A78" s="11"/>
@@ -7649,8 +7733,8 @@
       <c r="H78" s="14"/>
       <c r="I78" s="14"/>
       <c r="J78" s="15"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="24"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="22"/>
     </row>
     <row r="79" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A79" s="11"/>
@@ -7663,8 +7747,8 @@
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
       <c r="J79" s="15"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="24"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="22"/>
     </row>
     <row r="80" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A80" s="11"/>
@@ -7677,8 +7761,8 @@
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
       <c r="J80" s="15"/>
-      <c r="K80" s="23"/>
-      <c r="L80" s="24"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="22"/>
     </row>
     <row r="81" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A81" s="11"/>
@@ -7691,8 +7775,8 @@
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="15"/>
-      <c r="K81" s="23"/>
-      <c r="L81" s="24"/>
+      <c r="K81" s="21"/>
+      <c r="L81" s="22"/>
     </row>
     <row r="82" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A82" s="11"/>
@@ -7705,8 +7789,8 @@
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="15"/>
-      <c r="K82" s="23"/>
-      <c r="L82" s="24"/>
+      <c r="K82" s="21"/>
+      <c r="L82" s="22"/>
     </row>
     <row r="83" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A83" s="11"/>
@@ -7719,8 +7803,8 @@
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
       <c r="J83" s="15"/>
-      <c r="K83" s="23"/>
-      <c r="L83" s="24"/>
+      <c r="K83" s="21"/>
+      <c r="L83" s="22"/>
     </row>
     <row r="84" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A84" s="11"/>
@@ -7733,8 +7817,8 @@
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
       <c r="J84" s="15"/>
-      <c r="K84" s="23"/>
-      <c r="L84" s="24"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="22"/>
     </row>
     <row r="85" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A85" s="11"/>
@@ -7747,8 +7831,8 @@
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
       <c r="J85" s="15"/>
-      <c r="K85" s="23"/>
-      <c r="L85" s="24"/>
+      <c r="K85" s="21"/>
+      <c r="L85" s="22"/>
     </row>
     <row r="86" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A86" s="11"/>
@@ -7761,8 +7845,8 @@
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
       <c r="J86" s="15"/>
-      <c r="K86" s="23"/>
-      <c r="L86" s="24"/>
+      <c r="K86" s="21"/>
+      <c r="L86" s="22"/>
     </row>
     <row r="87" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A87" s="11"/>
@@ -7775,8 +7859,8 @@
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="15"/>
-      <c r="K87" s="23"/>
-      <c r="L87" s="24"/>
+      <c r="K87" s="21"/>
+      <c r="L87" s="22"/>
     </row>
     <row r="88" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A88" s="11"/>
@@ -7789,8 +7873,8 @@
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
       <c r="J88" s="15"/>
-      <c r="K88" s="23"/>
-      <c r="L88" s="24"/>
+      <c r="K88" s="21"/>
+      <c r="L88" s="22"/>
     </row>
     <row r="89" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A89" s="11"/>
@@ -7803,8 +7887,8 @@
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="15"/>
-      <c r="K89" s="23"/>
-      <c r="L89" s="24"/>
+      <c r="K89" s="21"/>
+      <c r="L89" s="22"/>
     </row>
     <row r="90" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A90" s="11"/>
@@ -7817,8 +7901,8 @@
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="15"/>
-      <c r="K90" s="23"/>
-      <c r="L90" s="24"/>
+      <c r="K90" s="21"/>
+      <c r="L90" s="22"/>
     </row>
     <row r="91" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A91" s="11"/>
@@ -7831,8 +7915,8 @@
       <c r="H91" s="14"/>
       <c r="I91" s="14"/>
       <c r="J91" s="15"/>
-      <c r="K91" s="23"/>
-      <c r="L91" s="24"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="22"/>
     </row>
     <row r="92" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A92" s="11"/>
@@ -7845,8 +7929,8 @@
       <c r="H92" s="14"/>
       <c r="I92" s="14"/>
       <c r="J92" s="15"/>
-      <c r="K92" s="23"/>
-      <c r="L92" s="24"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="22"/>
     </row>
     <row r="93" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A93" s="11"/>
@@ -7859,8 +7943,8 @@
       <c r="H93" s="14"/>
       <c r="I93" s="14"/>
       <c r="J93" s="15"/>
-      <c r="K93" s="23"/>
-      <c r="L93" s="24"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="22"/>
     </row>
     <row r="94" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A94" s="11"/>
@@ -7873,8 +7957,8 @@
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
       <c r="J94" s="15"/>
-      <c r="K94" s="23"/>
-      <c r="L94" s="24"/>
+      <c r="K94" s="21"/>
+      <c r="L94" s="22"/>
     </row>
     <row r="95" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A95" s="11"/>
@@ -7887,8 +7971,8 @@
       <c r="H95" s="14"/>
       <c r="I95" s="14"/>
       <c r="J95" s="15"/>
-      <c r="K95" s="23"/>
-      <c r="L95" s="24"/>
+      <c r="K95" s="21"/>
+      <c r="L95" s="22"/>
     </row>
     <row r="96" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A96" s="11"/>
@@ -7901,8 +7985,8 @@
       <c r="H96" s="14"/>
       <c r="I96" s="14"/>
       <c r="J96" s="15"/>
-      <c r="K96" s="23"/>
-      <c r="L96" s="24"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="22"/>
     </row>
     <row r="97" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A97" s="11"/>
@@ -7915,8 +7999,8 @@
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>
       <c r="J97" s="15"/>
-      <c r="K97" s="23"/>
-      <c r="L97" s="24"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="22"/>
     </row>
     <row r="98" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A98" s="11"/>
@@ -7929,8 +8013,8 @@
       <c r="H98" s="14"/>
       <c r="I98" s="14"/>
       <c r="J98" s="15"/>
-      <c r="K98" s="23"/>
-      <c r="L98" s="24"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="22"/>
     </row>
     <row r="99" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A99" s="11"/>
@@ -7943,8 +8027,8 @@
       <c r="H99" s="14"/>
       <c r="I99" s="14"/>
       <c r="J99" s="15"/>
-      <c r="K99" s="23"/>
-      <c r="L99" s="24"/>
+      <c r="K99" s="21"/>
+      <c r="L99" s="22"/>
     </row>
     <row r="100" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A100" s="11"/>
@@ -7957,8 +8041,8 @@
       <c r="H100" s="14"/>
       <c r="I100" s="14"/>
       <c r="J100" s="15"/>
-      <c r="K100" s="23"/>
-      <c r="L100" s="24"/>
+      <c r="K100" s="21"/>
+      <c r="L100" s="22"/>
     </row>
     <row r="101" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A101" s="11"/>
@@ -7971,8 +8055,8 @@
       <c r="H101" s="14"/>
       <c r="I101" s="14"/>
       <c r="J101" s="15"/>
-      <c r="K101" s="23"/>
-      <c r="L101" s="24"/>
+      <c r="K101" s="21"/>
+      <c r="L101" s="22"/>
     </row>
     <row r="102" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A102" s="11"/>
@@ -7985,8 +8069,8 @@
       <c r="H102" s="14"/>
       <c r="I102" s="14"/>
       <c r="J102" s="15"/>
-      <c r="K102" s="23"/>
-      <c r="L102" s="24"/>
+      <c r="K102" s="21"/>
+      <c r="L102" s="22"/>
     </row>
     <row r="103" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A103" s="11"/>
@@ -7999,8 +8083,8 @@
       <c r="H103" s="14"/>
       <c r="I103" s="14"/>
       <c r="J103" s="15"/>
-      <c r="K103" s="23"/>
-      <c r="L103" s="24"/>
+      <c r="K103" s="21"/>
+      <c r="L103" s="22"/>
     </row>
     <row r="104" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A104" s="11"/>
@@ -8013,8 +8097,8 @@
       <c r="H104" s="14"/>
       <c r="I104" s="14"/>
       <c r="J104" s="15"/>
-      <c r="K104" s="23"/>
-      <c r="L104" s="24"/>
+      <c r="K104" s="21"/>
+      <c r="L104" s="22"/>
     </row>
     <row r="105" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A105" s="11"/>
@@ -8027,8 +8111,8 @@
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
       <c r="J105" s="15"/>
-      <c r="K105" s="23"/>
-      <c r="L105" s="24"/>
+      <c r="K105" s="21"/>
+      <c r="L105" s="22"/>
     </row>
     <row r="106" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A106" s="11"/>
@@ -8041,8 +8125,8 @@
       <c r="H106" s="14"/>
       <c r="I106" s="14"/>
       <c r="J106" s="15"/>
-      <c r="K106" s="23"/>
-      <c r="L106" s="24"/>
+      <c r="K106" s="21"/>
+      <c r="L106" s="22"/>
     </row>
     <row r="107" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A107" s="11"/>
@@ -8055,8 +8139,8 @@
       <c r="H107" s="14"/>
       <c r="I107" s="14"/>
       <c r="J107" s="15"/>
-      <c r="K107" s="23"/>
-      <c r="L107" s="24"/>
+      <c r="K107" s="21"/>
+      <c r="L107" s="22"/>
     </row>
     <row r="108" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A108" s="11"/>
@@ -8069,8 +8153,8 @@
       <c r="H108" s="14"/>
       <c r="I108" s="14"/>
       <c r="J108" s="15"/>
-      <c r="K108" s="23"/>
-      <c r="L108" s="24"/>
+      <c r="K108" s="21"/>
+      <c r="L108" s="22"/>
     </row>
     <row r="109" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A109" s="11"/>
@@ -8083,8 +8167,8 @@
       <c r="H109" s="14"/>
       <c r="I109" s="14"/>
       <c r="J109" s="15"/>
-      <c r="K109" s="23"/>
-      <c r="L109" s="24"/>
+      <c r="K109" s="21"/>
+      <c r="L109" s="22"/>
     </row>
     <row r="110" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A110" s="11"/>
@@ -8097,8 +8181,8 @@
       <c r="H110" s="14"/>
       <c r="I110" s="14"/>
       <c r="J110" s="15"/>
-      <c r="K110" s="23"/>
-      <c r="L110" s="24"/>
+      <c r="K110" s="21"/>
+      <c r="L110" s="22"/>
     </row>
     <row r="111" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A111" s="11"/>
@@ -8111,8 +8195,8 @@
       <c r="H111" s="14"/>
       <c r="I111" s="14"/>
       <c r="J111" s="15"/>
-      <c r="K111" s="23"/>
-      <c r="L111" s="24"/>
+      <c r="K111" s="21"/>
+      <c r="L111" s="22"/>
     </row>
     <row r="112" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A112" s="11"/>
@@ -8125,8 +8209,8 @@
       <c r="H112" s="14"/>
       <c r="I112" s="14"/>
       <c r="J112" s="15"/>
-      <c r="K112" s="23"/>
-      <c r="L112" s="24"/>
+      <c r="K112" s="21"/>
+      <c r="L112" s="22"/>
     </row>
     <row r="113" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A113" s="11"/>
@@ -8139,8 +8223,8 @@
       <c r="H113" s="14"/>
       <c r="I113" s="14"/>
       <c r="J113" s="15"/>
-      <c r="K113" s="23"/>
-      <c r="L113" s="24"/>
+      <c r="K113" s="21"/>
+      <c r="L113" s="22"/>
     </row>
     <row r="114" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A114" s="11"/>
@@ -8153,8 +8237,8 @@
       <c r="H114" s="14"/>
       <c r="I114" s="14"/>
       <c r="J114" s="15"/>
-      <c r="K114" s="23"/>
-      <c r="L114" s="24"/>
+      <c r="K114" s="21"/>
+      <c r="L114" s="22"/>
     </row>
     <row r="115" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A115" s="11"/>
@@ -8167,8 +8251,8 @@
       <c r="H115" s="14"/>
       <c r="I115" s="14"/>
       <c r="J115" s="15"/>
-      <c r="K115" s="23"/>
-      <c r="L115" s="24"/>
+      <c r="K115" s="21"/>
+      <c r="L115" s="22"/>
     </row>
     <row r="116" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A116" s="11"/>
@@ -8181,8 +8265,8 @@
       <c r="H116" s="14"/>
       <c r="I116" s="14"/>
       <c r="J116" s="15"/>
-      <c r="K116" s="23"/>
-      <c r="L116" s="24"/>
+      <c r="K116" s="21"/>
+      <c r="L116" s="22"/>
     </row>
     <row r="117" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A117" s="11"/>
@@ -8195,8 +8279,8 @@
       <c r="H117" s="14"/>
       <c r="I117" s="14"/>
       <c r="J117" s="15"/>
-      <c r="K117" s="23"/>
-      <c r="L117" s="24"/>
+      <c r="K117" s="21"/>
+      <c r="L117" s="22"/>
     </row>
     <row r="118" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A118" s="11"/>
@@ -8209,8 +8293,8 @@
       <c r="H118" s="14"/>
       <c r="I118" s="14"/>
       <c r="J118" s="15"/>
-      <c r="K118" s="23"/>
-      <c r="L118" s="24"/>
+      <c r="K118" s="21"/>
+      <c r="L118" s="22"/>
     </row>
     <row r="119" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A119" s="11"/>
@@ -8223,8 +8307,8 @@
       <c r="H119" s="14"/>
       <c r="I119" s="14"/>
       <c r="J119" s="15"/>
-      <c r="K119" s="23"/>
-      <c r="L119" s="24"/>
+      <c r="K119" s="21"/>
+      <c r="L119" s="22"/>
     </row>
     <row r="120" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A120" s="11"/>
@@ -8237,8 +8321,8 @@
       <c r="H120" s="14"/>
       <c r="I120" s="14"/>
       <c r="J120" s="15"/>
-      <c r="K120" s="23"/>
-      <c r="L120" s="24"/>
+      <c r="K120" s="21"/>
+      <c r="L120" s="22"/>
     </row>
     <row r="121" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A121" s="11"/>
@@ -8251,8 +8335,8 @@
       <c r="H121" s="14"/>
       <c r="I121" s="14"/>
       <c r="J121" s="15"/>
-      <c r="K121" s="23"/>
-      <c r="L121" s="24"/>
+      <c r="K121" s="21"/>
+      <c r="L121" s="22"/>
     </row>
     <row r="122" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A122" s="11"/>
@@ -8265,8 +8349,8 @@
       <c r="H122" s="14"/>
       <c r="I122" s="14"/>
       <c r="J122" s="15"/>
-      <c r="K122" s="23"/>
-      <c r="L122" s="24"/>
+      <c r="K122" s="21"/>
+      <c r="L122" s="22"/>
     </row>
     <row r="123" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A123" s="11"/>
@@ -8279,8 +8363,8 @@
       <c r="H123" s="14"/>
       <c r="I123" s="14"/>
       <c r="J123" s="15"/>
-      <c r="K123" s="23"/>
-      <c r="L123" s="24"/>
+      <c r="K123" s="21"/>
+      <c r="L123" s="22"/>
     </row>
     <row r="124" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A124" s="11"/>
@@ -8293,8 +8377,8 @@
       <c r="H124" s="14"/>
       <c r="I124" s="14"/>
       <c r="J124" s="15"/>
-      <c r="K124" s="23"/>
-      <c r="L124" s="24"/>
+      <c r="K124" s="21"/>
+      <c r="L124" s="22"/>
     </row>
     <row r="125" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A125" s="11"/>
@@ -8307,8 +8391,8 @@
       <c r="H125" s="14"/>
       <c r="I125" s="14"/>
       <c r="J125" s="15"/>
-      <c r="K125" s="23"/>
-      <c r="L125" s="24"/>
+      <c r="K125" s="21"/>
+      <c r="L125" s="22"/>
     </row>
     <row r="126" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A126" s="11"/>
@@ -8321,8 +8405,8 @@
       <c r="H126" s="14"/>
       <c r="I126" s="14"/>
       <c r="J126" s="15"/>
-      <c r="K126" s="23"/>
-      <c r="L126" s="24"/>
+      <c r="K126" s="21"/>
+      <c r="L126" s="22"/>
     </row>
     <row r="127" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A127" s="11"/>
@@ -8335,8 +8419,8 @@
       <c r="H127" s="14"/>
       <c r="I127" s="14"/>
       <c r="J127" s="15"/>
-      <c r="K127" s="23"/>
-      <c r="L127" s="24"/>
+      <c r="K127" s="21"/>
+      <c r="L127" s="22"/>
     </row>
     <row r="128" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A128" s="11"/>
@@ -8349,8 +8433,8 @@
       <c r="H128" s="14"/>
       <c r="I128" s="14"/>
       <c r="J128" s="15"/>
-      <c r="K128" s="23"/>
-      <c r="L128" s="24"/>
+      <c r="K128" s="21"/>
+      <c r="L128" s="22"/>
     </row>
     <row r="129" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A129" s="11"/>
@@ -8363,8 +8447,8 @@
       <c r="H129" s="14"/>
       <c r="I129" s="14"/>
       <c r="J129" s="15"/>
-      <c r="K129" s="23"/>
-      <c r="L129" s="24"/>
+      <c r="K129" s="21"/>
+      <c r="L129" s="22"/>
     </row>
     <row r="130" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A130" s="11"/>
@@ -8377,8 +8461,8 @@
       <c r="H130" s="14"/>
       <c r="I130" s="14"/>
       <c r="J130" s="15"/>
-      <c r="K130" s="23"/>
-      <c r="L130" s="24"/>
+      <c r="K130" s="21"/>
+      <c r="L130" s="22"/>
     </row>
     <row r="131" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A131" s="11"/>
@@ -8391,8 +8475,8 @@
       <c r="H131" s="14"/>
       <c r="I131" s="14"/>
       <c r="J131" s="15"/>
-      <c r="K131" s="23"/>
-      <c r="L131" s="24"/>
+      <c r="K131" s="21"/>
+      <c r="L131" s="22"/>
     </row>
     <row r="132" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A132" s="11"/>
@@ -8405,8 +8489,8 @@
       <c r="H132" s="14"/>
       <c r="I132" s="14"/>
       <c r="J132" s="15"/>
-      <c r="K132" s="23"/>
-      <c r="L132" s="24"/>
+      <c r="K132" s="21"/>
+      <c r="L132" s="22"/>
     </row>
     <row r="133" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A133" s="11"/>
@@ -8419,8 +8503,8 @@
       <c r="H133" s="14"/>
       <c r="I133" s="14"/>
       <c r="J133" s="15"/>
-      <c r="K133" s="23"/>
-      <c r="L133" s="24"/>
+      <c r="K133" s="21"/>
+      <c r="L133" s="22"/>
     </row>
     <row r="134" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A134" s="11"/>
@@ -8433,8 +8517,8 @@
       <c r="H134" s="14"/>
       <c r="I134" s="14"/>
       <c r="J134" s="15"/>
-      <c r="K134" s="23"/>
-      <c r="L134" s="24"/>
+      <c r="K134" s="21"/>
+      <c r="L134" s="22"/>
     </row>
     <row r="135" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A135" s="11"/>
@@ -8447,8 +8531,8 @@
       <c r="H135" s="14"/>
       <c r="I135" s="14"/>
       <c r="J135" s="15"/>
-      <c r="K135" s="23"/>
-      <c r="L135" s="24"/>
+      <c r="K135" s="21"/>
+      <c r="L135" s="22"/>
     </row>
     <row r="136" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A136" s="11"/>
@@ -8461,8 +8545,8 @@
       <c r="H136" s="14"/>
       <c r="I136" s="14"/>
       <c r="J136" s="15"/>
-      <c r="K136" s="23"/>
-      <c r="L136" s="24"/>
+      <c r="K136" s="21"/>
+      <c r="L136" s="22"/>
     </row>
     <row r="137" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A137" s="11"/>
@@ -8475,8 +8559,8 @@
       <c r="H137" s="14"/>
       <c r="I137" s="14"/>
       <c r="J137" s="15"/>
-      <c r="K137" s="23"/>
-      <c r="L137" s="24"/>
+      <c r="K137" s="21"/>
+      <c r="L137" s="22"/>
     </row>
     <row r="138" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A138" s="11"/>
@@ -8489,8 +8573,8 @@
       <c r="H138" s="14"/>
       <c r="I138" s="14"/>
       <c r="J138" s="15"/>
-      <c r="K138" s="23"/>
-      <c r="L138" s="24"/>
+      <c r="K138" s="21"/>
+      <c r="L138" s="22"/>
     </row>
     <row r="139" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A139" s="11"/>
@@ -8503,8 +8587,8 @@
       <c r="H139" s="14"/>
       <c r="I139" s="14"/>
       <c r="J139" s="15"/>
-      <c r="K139" s="23"/>
-      <c r="L139" s="24"/>
+      <c r="K139" s="21"/>
+      <c r="L139" s="22"/>
     </row>
     <row r="140" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A140" s="11"/>
@@ -8517,8 +8601,8 @@
       <c r="H140" s="14"/>
       <c r="I140" s="14"/>
       <c r="J140" s="15"/>
-      <c r="K140" s="23"/>
-      <c r="L140" s="24"/>
+      <c r="K140" s="21"/>
+      <c r="L140" s="22"/>
     </row>
     <row r="141" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A141" s="11"/>
@@ -8531,8 +8615,8 @@
       <c r="H141" s="14"/>
       <c r="I141" s="14"/>
       <c r="J141" s="15"/>
-      <c r="K141" s="23"/>
-      <c r="L141" s="24"/>
+      <c r="K141" s="21"/>
+      <c r="L141" s="22"/>
     </row>
     <row r="142" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A142" s="11"/>
@@ -8545,8 +8629,8 @@
       <c r="H142" s="14"/>
       <c r="I142" s="14"/>
       <c r="J142" s="15"/>
-      <c r="K142" s="23"/>
-      <c r="L142" s="24"/>
+      <c r="K142" s="21"/>
+      <c r="L142" s="22"/>
     </row>
     <row r="143" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A143" s="11"/>
@@ -8559,8 +8643,8 @@
       <c r="H143" s="14"/>
       <c r="I143" s="14"/>
       <c r="J143" s="15"/>
-      <c r="K143" s="23"/>
-      <c r="L143" s="24"/>
+      <c r="K143" s="21"/>
+      <c r="L143" s="22"/>
     </row>
     <row r="144" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A144" s="11"/>
@@ -8573,8 +8657,8 @@
       <c r="H144" s="14"/>
       <c r="I144" s="14"/>
       <c r="J144" s="15"/>
-      <c r="K144" s="23"/>
-      <c r="L144" s="24"/>
+      <c r="K144" s="21"/>
+      <c r="L144" s="22"/>
     </row>
     <row r="145" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A145" s="11"/>
@@ -8587,8 +8671,8 @@
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
       <c r="J145" s="15"/>
-      <c r="K145" s="23"/>
-      <c r="L145" s="24"/>
+      <c r="K145" s="21"/>
+      <c r="L145" s="22"/>
     </row>
     <row r="146" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A146" s="11"/>
@@ -8601,8 +8685,8 @@
       <c r="H146" s="14"/>
       <c r="I146" s="14"/>
       <c r="J146" s="15"/>
-      <c r="K146" s="23"/>
-      <c r="L146" s="24"/>
+      <c r="K146" s="21"/>
+      <c r="L146" s="22"/>
     </row>
     <row r="147" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A147" s="11"/>
@@ -8615,8 +8699,8 @@
       <c r="H147" s="14"/>
       <c r="I147" s="14"/>
       <c r="J147" s="15"/>
-      <c r="K147" s="23"/>
-      <c r="L147" s="24"/>
+      <c r="K147" s="21"/>
+      <c r="L147" s="22"/>
     </row>
     <row r="148" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A148" s="11"/>
@@ -8629,8 +8713,8 @@
       <c r="H148" s="14"/>
       <c r="I148" s="14"/>
       <c r="J148" s="15"/>
-      <c r="K148" s="23"/>
-      <c r="L148" s="24"/>
+      <c r="K148" s="21"/>
+      <c r="L148" s="22"/>
     </row>
     <row r="149" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A149" s="11"/>
@@ -8643,8 +8727,8 @@
       <c r="H149" s="14"/>
       <c r="I149" s="14"/>
       <c r="J149" s="15"/>
-      <c r="K149" s="23"/>
-      <c r="L149" s="24"/>
+      <c r="K149" s="21"/>
+      <c r="L149" s="22"/>
     </row>
     <row r="150" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A150" s="11"/>
@@ -8657,8 +8741,8 @@
       <c r="H150" s="14"/>
       <c r="I150" s="14"/>
       <c r="J150" s="15"/>
-      <c r="K150" s="23"/>
-      <c r="L150" s="24"/>
+      <c r="K150" s="21"/>
+      <c r="L150" s="22"/>
     </row>
     <row r="151" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A151" s="11"/>
@@ -8671,8 +8755,8 @@
       <c r="H151" s="14"/>
       <c r="I151" s="14"/>
       <c r="J151" s="15"/>
-      <c r="K151" s="23"/>
-      <c r="L151" s="24"/>
+      <c r="K151" s="21"/>
+      <c r="L151" s="22"/>
     </row>
     <row r="152" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A152" s="11"/>
@@ -8685,8 +8769,8 @@
       <c r="H152" s="14"/>
       <c r="I152" s="14"/>
       <c r="J152" s="15"/>
-      <c r="K152" s="23"/>
-      <c r="L152" s="24"/>
+      <c r="K152" s="21"/>
+      <c r="L152" s="22"/>
     </row>
     <row r="153" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A153" s="11"/>
@@ -8699,8 +8783,8 @@
       <c r="H153" s="14"/>
       <c r="I153" s="14"/>
       <c r="J153" s="15"/>
-      <c r="K153" s="23"/>
-      <c r="L153" s="24"/>
+      <c r="K153" s="21"/>
+      <c r="L153" s="22"/>
     </row>
     <row r="154" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A154" s="11"/>
@@ -8713,8 +8797,8 @@
       <c r="H154" s="14"/>
       <c r="I154" s="14"/>
       <c r="J154" s="15"/>
-      <c r="K154" s="23"/>
-      <c r="L154" s="24"/>
+      <c r="K154" s="21"/>
+      <c r="L154" s="22"/>
     </row>
     <row r="155" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A155" s="11"/>
@@ -8727,8 +8811,8 @@
       <c r="H155" s="14"/>
       <c r="I155" s="14"/>
       <c r="J155" s="15"/>
-      <c r="K155" s="23"/>
-      <c r="L155" s="24"/>
+      <c r="K155" s="21"/>
+      <c r="L155" s="22"/>
     </row>
     <row r="156" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A156" s="11"/>
@@ -8741,8 +8825,8 @@
       <c r="H156" s="14"/>
       <c r="I156" s="14"/>
       <c r="J156" s="15"/>
-      <c r="K156" s="23"/>
-      <c r="L156" s="24"/>
+      <c r="K156" s="21"/>
+      <c r="L156" s="22"/>
     </row>
     <row r="157" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A157" s="11"/>
@@ -8755,8 +8839,8 @@
       <c r="H157" s="14"/>
       <c r="I157" s="14"/>
       <c r="J157" s="15"/>
-      <c r="K157" s="23"/>
-      <c r="L157" s="24"/>
+      <c r="K157" s="21"/>
+      <c r="L157" s="22"/>
     </row>
     <row r="158" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A158" s="11"/>
@@ -8769,8 +8853,8 @@
       <c r="H158" s="14"/>
       <c r="I158" s="14"/>
       <c r="J158" s="15"/>
-      <c r="K158" s="23"/>
-      <c r="L158" s="24"/>
+      <c r="K158" s="21"/>
+      <c r="L158" s="22"/>
     </row>
     <row r="159" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A159" s="11"/>
@@ -8783,8 +8867,8 @@
       <c r="H159" s="14"/>
       <c r="I159" s="14"/>
       <c r="J159" s="15"/>
-      <c r="K159" s="23"/>
-      <c r="L159" s="24"/>
+      <c r="K159" s="21"/>
+      <c r="L159" s="22"/>
     </row>
     <row r="160" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A160" s="11"/>
@@ -8797,8 +8881,8 @@
       <c r="H160" s="14"/>
       <c r="I160" s="14"/>
       <c r="J160" s="15"/>
-      <c r="K160" s="23"/>
-      <c r="L160" s="24"/>
+      <c r="K160" s="21"/>
+      <c r="L160" s="22"/>
     </row>
     <row r="161" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A161" s="11"/>
@@ -8811,8 +8895,8 @@
       <c r="H161" s="14"/>
       <c r="I161" s="14"/>
       <c r="J161" s="15"/>
-      <c r="K161" s="23"/>
-      <c r="L161" s="24"/>
+      <c r="K161" s="21"/>
+      <c r="L161" s="22"/>
     </row>
     <row r="162" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A162" s="11"/>
@@ -8825,8 +8909,8 @@
       <c r="H162" s="14"/>
       <c r="I162" s="14"/>
       <c r="J162" s="15"/>
-      <c r="K162" s="23"/>
-      <c r="L162" s="24"/>
+      <c r="K162" s="21"/>
+      <c r="L162" s="22"/>
     </row>
     <row r="163" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A163" s="11"/>
@@ -8839,8 +8923,8 @@
       <c r="H163" s="14"/>
       <c r="I163" s="14"/>
       <c r="J163" s="15"/>
-      <c r="K163" s="23"/>
-      <c r="L163" s="24"/>
+      <c r="K163" s="21"/>
+      <c r="L163" s="22"/>
     </row>
     <row r="164" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A164" s="11"/>
@@ -8853,8 +8937,8 @@
       <c r="H164" s="14"/>
       <c r="I164" s="14"/>
       <c r="J164" s="15"/>
-      <c r="K164" s="23"/>
-      <c r="L164" s="24"/>
+      <c r="K164" s="21"/>
+      <c r="L164" s="22"/>
     </row>
     <row r="165" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A165" s="11"/>
@@ -8867,8 +8951,8 @@
       <c r="H165" s="14"/>
       <c r="I165" s="14"/>
       <c r="J165" s="15"/>
-      <c r="K165" s="23"/>
-      <c r="L165" s="24"/>
+      <c r="K165" s="21"/>
+      <c r="L165" s="22"/>
     </row>
     <row r="166" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A166" s="11"/>
@@ -8881,8 +8965,8 @@
       <c r="H166" s="14"/>
       <c r="I166" s="14"/>
       <c r="J166" s="15"/>
-      <c r="K166" s="23"/>
-      <c r="L166" s="24"/>
+      <c r="K166" s="21"/>
+      <c r="L166" s="22"/>
     </row>
     <row r="167" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A167" s="11"/>
@@ -8895,8 +8979,8 @@
       <c r="H167" s="14"/>
       <c r="I167" s="14"/>
       <c r="J167" s="15"/>
-      <c r="K167" s="23"/>
-      <c r="L167" s="24"/>
+      <c r="K167" s="21"/>
+      <c r="L167" s="22"/>
     </row>
     <row r="168" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A168" s="11"/>
@@ -8909,8 +8993,8 @@
       <c r="H168" s="14"/>
       <c r="I168" s="14"/>
       <c r="J168" s="15"/>
-      <c r="K168" s="23"/>
-      <c r="L168" s="24"/>
+      <c r="K168" s="21"/>
+      <c r="L168" s="22"/>
     </row>
     <row r="169" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A169" s="11"/>
@@ -8923,8 +9007,8 @@
       <c r="H169" s="14"/>
       <c r="I169" s="14"/>
       <c r="J169" s="15"/>
-      <c r="K169" s="23"/>
-      <c r="L169" s="24"/>
+      <c r="K169" s="21"/>
+      <c r="L169" s="22"/>
     </row>
     <row r="170" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A170" s="11"/>
@@ -8937,8 +9021,8 @@
       <c r="H170" s="14"/>
       <c r="I170" s="14"/>
       <c r="J170" s="15"/>
-      <c r="K170" s="23"/>
-      <c r="L170" s="24"/>
+      <c r="K170" s="21"/>
+      <c r="L170" s="22"/>
     </row>
     <row r="171" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A171" s="11"/>
@@ -8951,8 +9035,8 @@
       <c r="H171" s="14"/>
       <c r="I171" s="14"/>
       <c r="J171" s="15"/>
-      <c r="K171" s="23"/>
-      <c r="L171" s="24"/>
+      <c r="K171" s="21"/>
+      <c r="L171" s="22"/>
     </row>
     <row r="172" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A172" s="11"/>
@@ -8965,8 +9049,8 @@
       <c r="H172" s="14"/>
       <c r="I172" s="14"/>
       <c r="J172" s="15"/>
-      <c r="K172" s="23"/>
-      <c r="L172" s="24"/>
+      <c r="K172" s="21"/>
+      <c r="L172" s="22"/>
     </row>
     <row r="173" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A173" s="11"/>
@@ -8979,8 +9063,8 @@
       <c r="H173" s="14"/>
       <c r="I173" s="14"/>
       <c r="J173" s="15"/>
-      <c r="K173" s="23"/>
-      <c r="L173" s="24"/>
+      <c r="K173" s="21"/>
+      <c r="L173" s="22"/>
     </row>
     <row r="174" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A174" s="11"/>
@@ -8993,8 +9077,8 @@
       <c r="H174" s="14"/>
       <c r="I174" s="14"/>
       <c r="J174" s="15"/>
-      <c r="K174" s="23"/>
-      <c r="L174" s="24"/>
+      <c r="K174" s="21"/>
+      <c r="L174" s="22"/>
     </row>
     <row r="175" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A175" s="11"/>
@@ -9007,8 +9091,8 @@
       <c r="H175" s="14"/>
       <c r="I175" s="14"/>
       <c r="J175" s="15"/>
-      <c r="K175" s="23"/>
-      <c r="L175" s="24"/>
+      <c r="K175" s="21"/>
+      <c r="L175" s="22"/>
     </row>
     <row r="176" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A176" s="11"/>
@@ -9021,8 +9105,8 @@
       <c r="H176" s="14"/>
       <c r="I176" s="14"/>
       <c r="J176" s="15"/>
-      <c r="K176" s="23"/>
-      <c r="L176" s="24"/>
+      <c r="K176" s="21"/>
+      <c r="L176" s="22"/>
     </row>
     <row r="177" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A177" s="11"/>
@@ -9035,8 +9119,8 @@
       <c r="H177" s="14"/>
       <c r="I177" s="14"/>
       <c r="J177" s="15"/>
-      <c r="K177" s="23"/>
-      <c r="L177" s="24"/>
+      <c r="K177" s="21"/>
+      <c r="L177" s="22"/>
     </row>
     <row r="178" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A178" s="11"/>
@@ -9049,8 +9133,8 @@
       <c r="H178" s="14"/>
       <c r="I178" s="14"/>
       <c r="J178" s="15"/>
-      <c r="K178" s="23"/>
-      <c r="L178" s="24"/>
+      <c r="K178" s="21"/>
+      <c r="L178" s="22"/>
     </row>
     <row r="179" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A179" s="11"/>
@@ -9063,8 +9147,8 @@
       <c r="H179" s="14"/>
       <c r="I179" s="14"/>
       <c r="J179" s="15"/>
-      <c r="K179" s="23"/>
-      <c r="L179" s="24"/>
+      <c r="K179" s="21"/>
+      <c r="L179" s="22"/>
     </row>
     <row r="180" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A180" s="11"/>
@@ -9077,8 +9161,8 @@
       <c r="H180" s="14"/>
       <c r="I180" s="14"/>
       <c r="J180" s="15"/>
-      <c r="K180" s="23"/>
-      <c r="L180" s="24"/>
+      <c r="K180" s="21"/>
+      <c r="L180" s="22"/>
     </row>
     <row r="181" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A181" s="11"/>
@@ -9091,8 +9175,8 @@
       <c r="H181" s="14"/>
       <c r="I181" s="14"/>
       <c r="J181" s="15"/>
-      <c r="K181" s="23"/>
-      <c r="L181" s="24"/>
+      <c r="K181" s="21"/>
+      <c r="L181" s="22"/>
     </row>
     <row r="182" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A182" s="11"/>
@@ -9105,8 +9189,8 @@
       <c r="H182" s="14"/>
       <c r="I182" s="14"/>
       <c r="J182" s="15"/>
-      <c r="K182" s="23"/>
-      <c r="L182" s="24"/>
+      <c r="K182" s="21"/>
+      <c r="L182" s="22"/>
     </row>
     <row r="183" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A183" s="11"/>
@@ -9119,8 +9203,8 @@
       <c r="H183" s="14"/>
       <c r="I183" s="14"/>
       <c r="J183" s="15"/>
-      <c r="K183" s="23"/>
-      <c r="L183" s="24"/>
+      <c r="K183" s="21"/>
+      <c r="L183" s="22"/>
     </row>
     <row r="184" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A184" s="11"/>
@@ -9133,8 +9217,8 @@
       <c r="H184" s="14"/>
       <c r="I184" s="14"/>
       <c r="J184" s="15"/>
-      <c r="K184" s="23"/>
-      <c r="L184" s="24"/>
+      <c r="K184" s="21"/>
+      <c r="L184" s="22"/>
     </row>
     <row r="185" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A185" s="11"/>
@@ -9147,8 +9231,8 @@
       <c r="H185" s="14"/>
       <c r="I185" s="14"/>
       <c r="J185" s="15"/>
-      <c r="K185" s="23"/>
-      <c r="L185" s="24"/>
+      <c r="K185" s="21"/>
+      <c r="L185" s="22"/>
     </row>
     <row r="186" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A186" s="11"/>
@@ -9161,8 +9245,8 @@
       <c r="H186" s="14"/>
       <c r="I186" s="14"/>
       <c r="J186" s="15"/>
-      <c r="K186" s="23"/>
-      <c r="L186" s="24"/>
+      <c r="K186" s="21"/>
+      <c r="L186" s="22"/>
     </row>
     <row r="187" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A187" s="11"/>
@@ -9175,8 +9259,8 @@
       <c r="H187" s="14"/>
       <c r="I187" s="14"/>
       <c r="J187" s="15"/>
-      <c r="K187" s="23"/>
-      <c r="L187" s="24"/>
+      <c r="K187" s="21"/>
+      <c r="L187" s="22"/>
     </row>
     <row r="188" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A188" s="11"/>
@@ -9189,8 +9273,8 @@
       <c r="H188" s="14"/>
       <c r="I188" s="14"/>
       <c r="J188" s="15"/>
-      <c r="K188" s="23"/>
-      <c r="L188" s="24"/>
+      <c r="K188" s="21"/>
+      <c r="L188" s="22"/>
     </row>
     <row r="189" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A189" s="11"/>
@@ -9203,8 +9287,8 @@
       <c r="H189" s="14"/>
       <c r="I189" s="14"/>
       <c r="J189" s="15"/>
-      <c r="K189" s="23"/>
-      <c r="L189" s="24"/>
+      <c r="K189" s="21"/>
+      <c r="L189" s="22"/>
     </row>
     <row r="190" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A190" s="11"/>
@@ -9217,8 +9301,8 @@
       <c r="H190" s="14"/>
       <c r="I190" s="14"/>
       <c r="J190" s="15"/>
-      <c r="K190" s="23"/>
-      <c r="L190" s="24"/>
+      <c r="K190" s="21"/>
+      <c r="L190" s="22"/>
     </row>
     <row r="191" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A191" s="11"/>
@@ -9231,8 +9315,8 @@
       <c r="H191" s="14"/>
       <c r="I191" s="14"/>
       <c r="J191" s="15"/>
-      <c r="K191" s="23"/>
-      <c r="L191" s="24"/>
+      <c r="K191" s="21"/>
+      <c r="L191" s="22"/>
     </row>
     <row r="192" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A192" s="11"/>
@@ -9245,8 +9329,8 @@
       <c r="H192" s="14"/>
       <c r="I192" s="14"/>
       <c r="J192" s="15"/>
-      <c r="K192" s="23"/>
-      <c r="L192" s="24"/>
+      <c r="K192" s="21"/>
+      <c r="L192" s="22"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
@@ -9306,15 +9390,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D5 D6 D9 D10 D11 D12 D13 D14 D15 D18 D19 D20 D21 D22 D23 D24 D25 D2:D3 D7:D8 D16:D17 D26:D192">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D5 D6 D9 D10 D11 D12 D13 D14 D15 D18 D19 D20 D21 D22 D23 D24 D27 D28 D29 D30 D31 D32 D33 D2:D3 D7:D8 D16:D17 D25:D26 D34:D192">
       <formula1>INDIRECT(C2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C11 C12 C13 C14 C15 C18 C19 C20 C21 C22 C23 C24 C25 C2:C3 C4:C5 C7:C8 C9:C10 C16:C17 C26:C192">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C11 C12 C13 C14 C15 C18 C19 C20 C21 C22 C23 C24 C27 C28 C29 C30 C31 C32 C33 C2:C3 C4:C5 C7:C8 C9:C10 C16:C17 C25:C26 C34:C192">
       <formula1>target</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E16" r:id="rId1" display="${uiurl}" tooltip="https://gnukhata.gitlab.io/gkapp/#/user-login"/>
+    <hyperlink ref="E25" r:id="rId1" display="${uiurl}" tooltip="https://gnukhata.gitlab.io/gkapp/#/user-login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
Updated Transfer note page
</commit_message>
<xml_diff>
--- a/tests/artifact/script/GNUKhata.macro.xlsx
+++ b/tests/artifact/script/GNUKhata.macro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6830" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="783">
   <si>
     <t>target</t>
   </si>
@@ -2438,6 +2438,12 @@
     <t>Given I maximize the browser window</t>
   </si>
   <si>
+    <t>resize the window</t>
+  </si>
+  <si>
+    <t>430</t>
+  </si>
+  <si>
     <t>${login.clickDefault}</t>
   </si>
   <si>
@@ -2483,14 +2489,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2525,6 +2531,18 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -2540,21 +2558,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -2563,18 +2566,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2587,6 +2606,37 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2594,15 +2644,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2616,55 +2667,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2679,6 +2683,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2705,7 +2723,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2717,7 +2735,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2729,7 +2753,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2741,19 +2861,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2765,127 +2903,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2915,16 +2933,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2944,37 +2980,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3005,161 +3021,163 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3211,6 +3229,22 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -3223,7 +3257,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3231,7 +3265,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3250,52 +3284,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -3617,7 +3651,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="18" width="8.33333333333333" customWidth="1" collapsed="1"/>
   </cols>
@@ -6285,15 +6319,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O192"/>
+  <dimension ref="A1:O193"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="$A24:$XFD24"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20.1666666666667" style="3" customWidth="1"/>
     <col min="2" max="2" width="31.5" style="4" customWidth="1"/>
@@ -6337,15 +6371,15 @@
       <c r="I1" s="10" t="s">
         <v>731</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="25" t="s">
         <v>732</v>
       </c>
-      <c r="K1" s="22"/>
+      <c r="K1" s="26"/>
       <c r="L1" s="10" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="41.4" spans="1:12">
+    <row r="2" s="2" customFormat="1" ht="42" spans="1:12">
       <c r="A2" s="11" t="s">
         <v>734</v>
       </c>
@@ -6368,8 +6402,8 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A3" s="11"/>
@@ -6390,8 +6424,8 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="28"/>
     </row>
     <row r="4" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A4" s="11"/>
@@ -6414,8 +6448,8 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="28"/>
     </row>
     <row r="5" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A5" s="11"/>
@@ -6436,10 +6470,10 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
-    </row>
-    <row r="6" s="2" customFormat="1" ht="41.4" spans="1:12">
+      <c r="K5" s="27"/>
+      <c r="L5" s="28"/>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="42" spans="1:12">
       <c r="A6" s="11" t="s">
         <v>744</v>
       </c>
@@ -6462,8 +6496,8 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="28"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="18" customHeight="1" spans="3:12">
       <c r="C7" s="13" t="s">
@@ -6482,8 +6516,8 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="28"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A8" s="11"/>
@@ -6504,8 +6538,8 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="28"/>
     </row>
     <row r="9" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A9" s="11"/>
@@ -6528,8 +6562,8 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="28"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A10" s="11"/>
@@ -6550,10 +6584,10 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-    </row>
-    <row r="11" s="2" customFormat="1" ht="96.6" spans="1:12">
+      <c r="K10" s="27"/>
+      <c r="L10" s="28"/>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="98" spans="1:12">
       <c r="A11" s="11" t="s">
         <v>750</v>
       </c>
@@ -6576,8 +6610,8 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="28"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A12" s="11"/>
@@ -6598,8 +6632,8 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="28"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A13" s="11"/>
@@ -6620,8 +6654,8 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="15"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="28"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A14" s="11"/>
@@ -6644,8 +6678,8 @@
       <c r="J14" s="15" t="s">
         <v>760</v>
       </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="28"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A15" s="11"/>
@@ -6664,10 +6698,10 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="27.6" spans="1:15">
+      <c r="K15" s="27"/>
+      <c r="L15" s="28"/>
+    </row>
+    <row r="16" s="2" customFormat="1" ht="28" spans="1:15">
       <c r="A16" s="11" t="s">
         <v>762</v>
       </c>
@@ -6690,11 +6724,11 @@
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="23"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="27"/>
     </row>
     <row r="17" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="11"/>
@@ -6711,88 +6745,90 @@
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="23"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="27"/>
     </row>
     <row r="18" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13" t="s">
+      <c r="B18" s="17" t="s">
+        <v>767</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>553</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>767</v>
-      </c>
-      <c r="F18" s="17">
-        <v>5000</v>
+      <c r="D18" s="19" t="s">
+        <v>640</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>768</v>
+      </c>
+      <c r="F18" s="20">
+        <v>932</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="23"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="27"/>
     </row>
     <row r="19" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="11"/>
-      <c r="B19" s="12" t="s">
-        <v>768</v>
-      </c>
+      <c r="B19" s="12"/>
       <c r="C19" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>363</v>
+        <v>553</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>767</v>
-      </c>
-      <c r="F19" s="14"/>
+        <v>769</v>
+      </c>
+      <c r="F19" s="21">
+        <v>5000</v>
+      </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="23"/>
-    </row>
-    <row r="20" s="2" customFormat="1" ht="22" customHeight="1" spans="1:15">
+      <c r="K19" s="27"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="27"/>
+    </row>
+    <row r="20" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A20" s="11"/>
       <c r="B20" s="12" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>713</v>
+        <v>363</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>770</v>
-      </c>
-      <c r="F20" s="15"/>
+        <v>769</v>
+      </c>
+      <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="15"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="23"/>
-    </row>
-    <row r="21" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
+      <c r="K20" s="27"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="27"/>
+    </row>
+    <row r="21" s="2" customFormat="1" ht="22" customHeight="1" spans="1:15">
       <c r="A21" s="11"/>
       <c r="B21" s="12" t="s">
         <v>771</v>
@@ -6801,28 +6837,26 @@
         <v>30</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>772</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>773</v>
-      </c>
+      <c r="F21" s="15"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="15"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="23"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="27"/>
     </row>
     <row r="22" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="11"/>
       <c r="B22" s="12" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>30</v>
@@ -6831,47 +6865,49 @@
         <v>705</v>
       </c>
       <c r="E22" s="14" t="s">
+        <v>774</v>
+      </c>
+      <c r="F22" s="14" t="s">
         <v>775</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>776</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="15"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="23"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="27"/>
     </row>
     <row r="23" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="11"/>
       <c r="B23" s="12" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>363</v>
+        <v>705</v>
       </c>
       <c r="E23" s="14" t="s">
+        <v>777</v>
+      </c>
+      <c r="F23" s="14" t="s">
         <v>778</v>
       </c>
-      <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="23"/>
-    </row>
-    <row r="24" s="2" customFormat="1" ht="19" customHeight="1" spans="1:15">
+      <c r="K23" s="27"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="27"/>
+    </row>
+    <row r="24" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A24" s="11"/>
       <c r="B24" s="12" t="s">
         <v>779</v>
@@ -6880,49 +6916,60 @@
         <v>30</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>559</v>
+        <v>363</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>780</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="23"/>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K24" s="27"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="27"/>
+    </row>
+    <row r="25" s="2" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="B25" s="12" t="s">
+        <v>781</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>782</v>
+      </c>
+      <c r="F25" s="15"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="27"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="24"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="28"/>
     </row>
     <row r="27" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A27" s="11"/>
@@ -6935,8 +6982,8 @@
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="15"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="24"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="28"/>
     </row>
     <row r="28" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A28" s="11"/>
@@ -6949,8 +6996,8 @@
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="15"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="24"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="28"/>
     </row>
     <row r="29" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A29" s="11"/>
@@ -6963,8 +7010,8 @@
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="24"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="28"/>
     </row>
     <row r="30" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A30" s="11"/>
@@ -6977,36 +7024,36 @@
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="15"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="24"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="28"/>
     </row>
     <row r="31" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="13"/>
       <c r="D31" s="14"/>
-      <c r="E31" s="20"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="15"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="24"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="28"/>
     </row>
     <row r="32" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="13"/>
       <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="E32" s="24"/>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="15"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="24"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="28"/>
     </row>
     <row r="33" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A33" s="11"/>
@@ -7019,8 +7066,8 @@
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="15"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="24"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="28"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A34" s="11"/>
@@ -7033,8 +7080,8 @@
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="15"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="24"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="28"/>
     </row>
     <row r="35" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A35" s="11"/>
@@ -7047,8 +7094,8 @@
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="15"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="24"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="28"/>
     </row>
     <row r="36" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A36" s="11"/>
@@ -7061,8 +7108,8 @@
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="15"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="24"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="28"/>
     </row>
     <row r="37" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A37" s="11"/>
@@ -7075,8 +7122,8 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="15"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="24"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="28"/>
     </row>
     <row r="38" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A38" s="11"/>
@@ -7089,8 +7136,8 @@
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="24"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="28"/>
     </row>
     <row r="39" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A39" s="11"/>
@@ -7103,8 +7150,8 @@
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="15"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="24"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="28"/>
     </row>
     <row r="40" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A40" s="11"/>
@@ -7117,8 +7164,8 @@
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="15"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="24"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="28"/>
     </row>
     <row r="41" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A41" s="11"/>
@@ -7131,8 +7178,8 @@
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="15"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="24"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="28"/>
     </row>
     <row r="42" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A42" s="11"/>
@@ -7145,8 +7192,8 @@
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="24"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="28"/>
     </row>
     <row r="43" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A43" s="11"/>
@@ -7159,8 +7206,8 @@
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="15"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="24"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="28"/>
     </row>
     <row r="44" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A44" s="11"/>
@@ -7173,8 +7220,8 @@
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="15"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="24"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="28"/>
     </row>
     <row r="45" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A45" s="11"/>
@@ -7187,8 +7234,8 @@
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="15"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="24"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="28"/>
     </row>
     <row r="46" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A46" s="11"/>
@@ -7201,8 +7248,8 @@
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="15"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="24"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="28"/>
     </row>
     <row r="47" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A47" s="11"/>
@@ -7215,8 +7262,8 @@
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="15"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="24"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="28"/>
     </row>
     <row r="48" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A48" s="11"/>
@@ -7229,8 +7276,8 @@
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="15"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="24"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="28"/>
     </row>
     <row r="49" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A49" s="11"/>
@@ -7243,8 +7290,8 @@
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="24"/>
+      <c r="K49" s="27"/>
+      <c r="L49" s="28"/>
     </row>
     <row r="50" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A50" s="11"/>
@@ -7257,8 +7304,8 @@
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
       <c r="J50" s="15"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="24"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="28"/>
     </row>
     <row r="51" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A51" s="11"/>
@@ -7271,8 +7318,8 @@
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
       <c r="J51" s="15"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="24"/>
+      <c r="K51" s="27"/>
+      <c r="L51" s="28"/>
     </row>
     <row r="52" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A52" s="11"/>
@@ -7285,8 +7332,8 @@
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
       <c r="J52" s="15"/>
-      <c r="K52" s="23"/>
-      <c r="L52" s="24"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="28"/>
     </row>
     <row r="53" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A53" s="11"/>
@@ -7299,8 +7346,8 @@
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
       <c r="J53" s="15"/>
-      <c r="K53" s="23"/>
-      <c r="L53" s="24"/>
+      <c r="K53" s="27"/>
+      <c r="L53" s="28"/>
     </row>
     <row r="54" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A54" s="11"/>
@@ -7313,8 +7360,8 @@
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
       <c r="J54" s="15"/>
-      <c r="K54" s="23"/>
-      <c r="L54" s="24"/>
+      <c r="K54" s="27"/>
+      <c r="L54" s="28"/>
     </row>
     <row r="55" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A55" s="11"/>
@@ -7327,8 +7374,8 @@
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
       <c r="J55" s="15"/>
-      <c r="K55" s="23"/>
-      <c r="L55" s="24"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="28"/>
     </row>
     <row r="56" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A56" s="11"/>
@@ -7341,8 +7388,8 @@
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
       <c r="J56" s="15"/>
-      <c r="K56" s="23"/>
-      <c r="L56" s="24"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="28"/>
     </row>
     <row r="57" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A57" s="11"/>
@@ -7355,8 +7402,8 @@
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
       <c r="J57" s="15"/>
-      <c r="K57" s="23"/>
-      <c r="L57" s="24"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="28"/>
     </row>
     <row r="58" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A58" s="11"/>
@@ -7369,8 +7416,8 @@
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
       <c r="J58" s="15"/>
-      <c r="K58" s="23"/>
-      <c r="L58" s="24"/>
+      <c r="K58" s="27"/>
+      <c r="L58" s="28"/>
     </row>
     <row r="59" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A59" s="11"/>
@@ -7383,8 +7430,8 @@
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
       <c r="J59" s="15"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="24"/>
+      <c r="K59" s="27"/>
+      <c r="L59" s="28"/>
     </row>
     <row r="60" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A60" s="11"/>
@@ -7397,8 +7444,8 @@
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
       <c r="J60" s="15"/>
-      <c r="K60" s="23"/>
-      <c r="L60" s="24"/>
+      <c r="K60" s="27"/>
+      <c r="L60" s="28"/>
     </row>
     <row r="61" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A61" s="11"/>
@@ -7411,8 +7458,8 @@
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
       <c r="J61" s="15"/>
-      <c r="K61" s="23"/>
-      <c r="L61" s="24"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="28"/>
     </row>
     <row r="62" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A62" s="11"/>
@@ -7425,8 +7472,8 @@
       <c r="H62" s="14"/>
       <c r="I62" s="14"/>
       <c r="J62" s="15"/>
-      <c r="K62" s="23"/>
-      <c r="L62" s="24"/>
+      <c r="K62" s="27"/>
+      <c r="L62" s="28"/>
     </row>
     <row r="63" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A63" s="11"/>
@@ -7439,8 +7486,8 @@
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
       <c r="J63" s="15"/>
-      <c r="K63" s="23"/>
-      <c r="L63" s="24"/>
+      <c r="K63" s="27"/>
+      <c r="L63" s="28"/>
     </row>
     <row r="64" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A64" s="11"/>
@@ -7453,8 +7500,8 @@
       <c r="H64" s="14"/>
       <c r="I64" s="14"/>
       <c r="J64" s="15"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="24"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="28"/>
     </row>
     <row r="65" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A65" s="11"/>
@@ -7467,8 +7514,8 @@
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
       <c r="J65" s="15"/>
-      <c r="K65" s="23"/>
-      <c r="L65" s="24"/>
+      <c r="K65" s="27"/>
+      <c r="L65" s="28"/>
     </row>
     <row r="66" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A66" s="11"/>
@@ -7481,8 +7528,8 @@
       <c r="H66" s="14"/>
       <c r="I66" s="14"/>
       <c r="J66" s="15"/>
-      <c r="K66" s="23"/>
-      <c r="L66" s="24"/>
+      <c r="K66" s="27"/>
+      <c r="L66" s="28"/>
     </row>
     <row r="67" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A67" s="11"/>
@@ -7495,8 +7542,8 @@
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
       <c r="J67" s="15"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="24"/>
+      <c r="K67" s="27"/>
+      <c r="L67" s="28"/>
     </row>
     <row r="68" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A68" s="11"/>
@@ -7509,8 +7556,8 @@
       <c r="H68" s="14"/>
       <c r="I68" s="14"/>
       <c r="J68" s="15"/>
-      <c r="K68" s="23"/>
-      <c r="L68" s="24"/>
+      <c r="K68" s="27"/>
+      <c r="L68" s="28"/>
     </row>
     <row r="69" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A69" s="11"/>
@@ -7523,8 +7570,8 @@
       <c r="H69" s="14"/>
       <c r="I69" s="14"/>
       <c r="J69" s="15"/>
-      <c r="K69" s="23"/>
-      <c r="L69" s="24"/>
+      <c r="K69" s="27"/>
+      <c r="L69" s="28"/>
     </row>
     <row r="70" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A70" s="11"/>
@@ -7537,8 +7584,8 @@
       <c r="H70" s="14"/>
       <c r="I70" s="14"/>
       <c r="J70" s="15"/>
-      <c r="K70" s="23"/>
-      <c r="L70" s="24"/>
+      <c r="K70" s="27"/>
+      <c r="L70" s="28"/>
     </row>
     <row r="71" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A71" s="11"/>
@@ -7551,8 +7598,8 @@
       <c r="H71" s="14"/>
       <c r="I71" s="14"/>
       <c r="J71" s="15"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="24"/>
+      <c r="K71" s="27"/>
+      <c r="L71" s="28"/>
     </row>
     <row r="72" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A72" s="11"/>
@@ -7565,8 +7612,8 @@
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
       <c r="J72" s="15"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="24"/>
+      <c r="K72" s="27"/>
+      <c r="L72" s="28"/>
     </row>
     <row r="73" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A73" s="11"/>
@@ -7579,8 +7626,8 @@
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
       <c r="J73" s="15"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="24"/>
+      <c r="K73" s="27"/>
+      <c r="L73" s="28"/>
     </row>
     <row r="74" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A74" s="11"/>
@@ -7593,8 +7640,8 @@
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
       <c r="J74" s="15"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="24"/>
+      <c r="K74" s="27"/>
+      <c r="L74" s="28"/>
     </row>
     <row r="75" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A75" s="11"/>
@@ -7607,8 +7654,8 @@
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
       <c r="J75" s="15"/>
-      <c r="K75" s="23"/>
-      <c r="L75" s="24"/>
+      <c r="K75" s="27"/>
+      <c r="L75" s="28"/>
     </row>
     <row r="76" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A76" s="11"/>
@@ -7621,8 +7668,8 @@
       <c r="H76" s="14"/>
       <c r="I76" s="14"/>
       <c r="J76" s="15"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="24"/>
+      <c r="K76" s="27"/>
+      <c r="L76" s="28"/>
     </row>
     <row r="77" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A77" s="11"/>
@@ -7635,8 +7682,8 @@
       <c r="H77" s="14"/>
       <c r="I77" s="14"/>
       <c r="J77" s="15"/>
-      <c r="K77" s="23"/>
-      <c r="L77" s="24"/>
+      <c r="K77" s="27"/>
+      <c r="L77" s="28"/>
     </row>
     <row r="78" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A78" s="11"/>
@@ -7649,8 +7696,8 @@
       <c r="H78" s="14"/>
       <c r="I78" s="14"/>
       <c r="J78" s="15"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="24"/>
+      <c r="K78" s="27"/>
+      <c r="L78" s="28"/>
     </row>
     <row r="79" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A79" s="11"/>
@@ -7663,8 +7710,8 @@
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
       <c r="J79" s="15"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="24"/>
+      <c r="K79" s="27"/>
+      <c r="L79" s="28"/>
     </row>
     <row r="80" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A80" s="11"/>
@@ -7677,8 +7724,8 @@
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
       <c r="J80" s="15"/>
-      <c r="K80" s="23"/>
-      <c r="L80" s="24"/>
+      <c r="K80" s="27"/>
+      <c r="L80" s="28"/>
     </row>
     <row r="81" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A81" s="11"/>
@@ -7691,8 +7738,8 @@
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="15"/>
-      <c r="K81" s="23"/>
-      <c r="L81" s="24"/>
+      <c r="K81" s="27"/>
+      <c r="L81" s="28"/>
     </row>
     <row r="82" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A82" s="11"/>
@@ -7705,8 +7752,8 @@
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="15"/>
-      <c r="K82" s="23"/>
-      <c r="L82" s="24"/>
+      <c r="K82" s="27"/>
+      <c r="L82" s="28"/>
     </row>
     <row r="83" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A83" s="11"/>
@@ -7719,8 +7766,8 @@
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
       <c r="J83" s="15"/>
-      <c r="K83" s="23"/>
-      <c r="L83" s="24"/>
+      <c r="K83" s="27"/>
+      <c r="L83" s="28"/>
     </row>
     <row r="84" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A84" s="11"/>
@@ -7733,8 +7780,8 @@
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
       <c r="J84" s="15"/>
-      <c r="K84" s="23"/>
-      <c r="L84" s="24"/>
+      <c r="K84" s="27"/>
+      <c r="L84" s="28"/>
     </row>
     <row r="85" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A85" s="11"/>
@@ -7747,8 +7794,8 @@
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
       <c r="J85" s="15"/>
-      <c r="K85" s="23"/>
-      <c r="L85" s="24"/>
+      <c r="K85" s="27"/>
+      <c r="L85" s="28"/>
     </row>
     <row r="86" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A86" s="11"/>
@@ -7761,8 +7808,8 @@
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
       <c r="J86" s="15"/>
-      <c r="K86" s="23"/>
-      <c r="L86" s="24"/>
+      <c r="K86" s="27"/>
+      <c r="L86" s="28"/>
     </row>
     <row r="87" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A87" s="11"/>
@@ -7775,8 +7822,8 @@
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="15"/>
-      <c r="K87" s="23"/>
-      <c r="L87" s="24"/>
+      <c r="K87" s="27"/>
+      <c r="L87" s="28"/>
     </row>
     <row r="88" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A88" s="11"/>
@@ -7789,8 +7836,8 @@
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
       <c r="J88" s="15"/>
-      <c r="K88" s="23"/>
-      <c r="L88" s="24"/>
+      <c r="K88" s="27"/>
+      <c r="L88" s="28"/>
     </row>
     <row r="89" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A89" s="11"/>
@@ -7803,8 +7850,8 @@
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="15"/>
-      <c r="K89" s="23"/>
-      <c r="L89" s="24"/>
+      <c r="K89" s="27"/>
+      <c r="L89" s="28"/>
     </row>
     <row r="90" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A90" s="11"/>
@@ -7817,8 +7864,8 @@
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="15"/>
-      <c r="K90" s="23"/>
-      <c r="L90" s="24"/>
+      <c r="K90" s="27"/>
+      <c r="L90" s="28"/>
     </row>
     <row r="91" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A91" s="11"/>
@@ -7831,8 +7878,8 @@
       <c r="H91" s="14"/>
       <c r="I91" s="14"/>
       <c r="J91" s="15"/>
-      <c r="K91" s="23"/>
-      <c r="L91" s="24"/>
+      <c r="K91" s="27"/>
+      <c r="L91" s="28"/>
     </row>
     <row r="92" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A92" s="11"/>
@@ -7845,10 +7892,10 @@
       <c r="H92" s="14"/>
       <c r="I92" s="14"/>
       <c r="J92" s="15"/>
-      <c r="K92" s="23"/>
-      <c r="L92" s="24"/>
-    </row>
-    <row r="93" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
+      <c r="K92" s="27"/>
+      <c r="L92" s="28"/>
+    </row>
+    <row r="93" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A93" s="11"/>
       <c r="B93" s="12"/>
       <c r="C93" s="13"/>
@@ -7859,8 +7906,8 @@
       <c r="H93" s="14"/>
       <c r="I93" s="14"/>
       <c r="J93" s="15"/>
-      <c r="K93" s="23"/>
-      <c r="L93" s="24"/>
+      <c r="K93" s="27"/>
+      <c r="L93" s="28"/>
     </row>
     <row r="94" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A94" s="11"/>
@@ -7873,8 +7920,8 @@
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
       <c r="J94" s="15"/>
-      <c r="K94" s="23"/>
-      <c r="L94" s="24"/>
+      <c r="K94" s="27"/>
+      <c r="L94" s="28"/>
     </row>
     <row r="95" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A95" s="11"/>
@@ -7887,8 +7934,8 @@
       <c r="H95" s="14"/>
       <c r="I95" s="14"/>
       <c r="J95" s="15"/>
-      <c r="K95" s="23"/>
-      <c r="L95" s="24"/>
+      <c r="K95" s="27"/>
+      <c r="L95" s="28"/>
     </row>
     <row r="96" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A96" s="11"/>
@@ -7901,8 +7948,8 @@
       <c r="H96" s="14"/>
       <c r="I96" s="14"/>
       <c r="J96" s="15"/>
-      <c r="K96" s="23"/>
-      <c r="L96" s="24"/>
+      <c r="K96" s="27"/>
+      <c r="L96" s="28"/>
     </row>
     <row r="97" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A97" s="11"/>
@@ -7915,8 +7962,8 @@
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>
       <c r="J97" s="15"/>
-      <c r="K97" s="23"/>
-      <c r="L97" s="24"/>
+      <c r="K97" s="27"/>
+      <c r="L97" s="28"/>
     </row>
     <row r="98" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A98" s="11"/>
@@ -7929,8 +7976,8 @@
       <c r="H98" s="14"/>
       <c r="I98" s="14"/>
       <c r="J98" s="15"/>
-      <c r="K98" s="23"/>
-      <c r="L98" s="24"/>
+      <c r="K98" s="27"/>
+      <c r="L98" s="28"/>
     </row>
     <row r="99" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A99" s="11"/>
@@ -7943,8 +7990,8 @@
       <c r="H99" s="14"/>
       <c r="I99" s="14"/>
       <c r="J99" s="15"/>
-      <c r="K99" s="23"/>
-      <c r="L99" s="24"/>
+      <c r="K99" s="27"/>
+      <c r="L99" s="28"/>
     </row>
     <row r="100" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A100" s="11"/>
@@ -7957,8 +8004,8 @@
       <c r="H100" s="14"/>
       <c r="I100" s="14"/>
       <c r="J100" s="15"/>
-      <c r="K100" s="23"/>
-      <c r="L100" s="24"/>
+      <c r="K100" s="27"/>
+      <c r="L100" s="28"/>
     </row>
     <row r="101" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A101" s="11"/>
@@ -7971,8 +8018,8 @@
       <c r="H101" s="14"/>
       <c r="I101" s="14"/>
       <c r="J101" s="15"/>
-      <c r="K101" s="23"/>
-      <c r="L101" s="24"/>
+      <c r="K101" s="27"/>
+      <c r="L101" s="28"/>
     </row>
     <row r="102" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A102" s="11"/>
@@ -7985,8 +8032,8 @@
       <c r="H102" s="14"/>
       <c r="I102" s="14"/>
       <c r="J102" s="15"/>
-      <c r="K102" s="23"/>
-      <c r="L102" s="24"/>
+      <c r="K102" s="27"/>
+      <c r="L102" s="28"/>
     </row>
     <row r="103" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A103" s="11"/>
@@ -7999,8 +8046,8 @@
       <c r="H103" s="14"/>
       <c r="I103" s="14"/>
       <c r="J103" s="15"/>
-      <c r="K103" s="23"/>
-      <c r="L103" s="24"/>
+      <c r="K103" s="27"/>
+      <c r="L103" s="28"/>
     </row>
     <row r="104" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A104" s="11"/>
@@ -8013,8 +8060,8 @@
       <c r="H104" s="14"/>
       <c r="I104" s="14"/>
       <c r="J104" s="15"/>
-      <c r="K104" s="23"/>
-      <c r="L104" s="24"/>
+      <c r="K104" s="27"/>
+      <c r="L104" s="28"/>
     </row>
     <row r="105" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A105" s="11"/>
@@ -8027,8 +8074,8 @@
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
       <c r="J105" s="15"/>
-      <c r="K105" s="23"/>
-      <c r="L105" s="24"/>
+      <c r="K105" s="27"/>
+      <c r="L105" s="28"/>
     </row>
     <row r="106" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A106" s="11"/>
@@ -8041,8 +8088,8 @@
       <c r="H106" s="14"/>
       <c r="I106" s="14"/>
       <c r="J106" s="15"/>
-      <c r="K106" s="23"/>
-      <c r="L106" s="24"/>
+      <c r="K106" s="27"/>
+      <c r="L106" s="28"/>
     </row>
     <row r="107" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A107" s="11"/>
@@ -8055,8 +8102,8 @@
       <c r="H107" s="14"/>
       <c r="I107" s="14"/>
       <c r="J107" s="15"/>
-      <c r="K107" s="23"/>
-      <c r="L107" s="24"/>
+      <c r="K107" s="27"/>
+      <c r="L107" s="28"/>
     </row>
     <row r="108" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A108" s="11"/>
@@ -8069,8 +8116,8 @@
       <c r="H108" s="14"/>
       <c r="I108" s="14"/>
       <c r="J108" s="15"/>
-      <c r="K108" s="23"/>
-      <c r="L108" s="24"/>
+      <c r="K108" s="27"/>
+      <c r="L108" s="28"/>
     </row>
     <row r="109" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A109" s="11"/>
@@ -8083,8 +8130,8 @@
       <c r="H109" s="14"/>
       <c r="I109" s="14"/>
       <c r="J109" s="15"/>
-      <c r="K109" s="23"/>
-      <c r="L109" s="24"/>
+      <c r="K109" s="27"/>
+      <c r="L109" s="28"/>
     </row>
     <row r="110" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A110" s="11"/>
@@ -8097,8 +8144,8 @@
       <c r="H110" s="14"/>
       <c r="I110" s="14"/>
       <c r="J110" s="15"/>
-      <c r="K110" s="23"/>
-      <c r="L110" s="24"/>
+      <c r="K110" s="27"/>
+      <c r="L110" s="28"/>
     </row>
     <row r="111" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A111" s="11"/>
@@ -8111,8 +8158,8 @@
       <c r="H111" s="14"/>
       <c r="I111" s="14"/>
       <c r="J111" s="15"/>
-      <c r="K111" s="23"/>
-      <c r="L111" s="24"/>
+      <c r="K111" s="27"/>
+      <c r="L111" s="28"/>
     </row>
     <row r="112" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A112" s="11"/>
@@ -8125,8 +8172,8 @@
       <c r="H112" s="14"/>
       <c r="I112" s="14"/>
       <c r="J112" s="15"/>
-      <c r="K112" s="23"/>
-      <c r="L112" s="24"/>
+      <c r="K112" s="27"/>
+      <c r="L112" s="28"/>
     </row>
     <row r="113" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A113" s="11"/>
@@ -8139,8 +8186,8 @@
       <c r="H113" s="14"/>
       <c r="I113" s="14"/>
       <c r="J113" s="15"/>
-      <c r="K113" s="23"/>
-      <c r="L113" s="24"/>
+      <c r="K113" s="27"/>
+      <c r="L113" s="28"/>
     </row>
     <row r="114" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A114" s="11"/>
@@ -8153,8 +8200,8 @@
       <c r="H114" s="14"/>
       <c r="I114" s="14"/>
       <c r="J114" s="15"/>
-      <c r="K114" s="23"/>
-      <c r="L114" s="24"/>
+      <c r="K114" s="27"/>
+      <c r="L114" s="28"/>
     </row>
     <row r="115" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A115" s="11"/>
@@ -8167,8 +8214,8 @@
       <c r="H115" s="14"/>
       <c r="I115" s="14"/>
       <c r="J115" s="15"/>
-      <c r="K115" s="23"/>
-      <c r="L115" s="24"/>
+      <c r="K115" s="27"/>
+      <c r="L115" s="28"/>
     </row>
     <row r="116" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A116" s="11"/>
@@ -8181,8 +8228,8 @@
       <c r="H116" s="14"/>
       <c r="I116" s="14"/>
       <c r="J116" s="15"/>
-      <c r="K116" s="23"/>
-      <c r="L116" s="24"/>
+      <c r="K116" s="27"/>
+      <c r="L116" s="28"/>
     </row>
     <row r="117" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A117" s="11"/>
@@ -8195,8 +8242,8 @@
       <c r="H117" s="14"/>
       <c r="I117" s="14"/>
       <c r="J117" s="15"/>
-      <c r="K117" s="23"/>
-      <c r="L117" s="24"/>
+      <c r="K117" s="27"/>
+      <c r="L117" s="28"/>
     </row>
     <row r="118" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A118" s="11"/>
@@ -8209,8 +8256,8 @@
       <c r="H118" s="14"/>
       <c r="I118" s="14"/>
       <c r="J118" s="15"/>
-      <c r="K118" s="23"/>
-      <c r="L118" s="24"/>
+      <c r="K118" s="27"/>
+      <c r="L118" s="28"/>
     </row>
     <row r="119" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A119" s="11"/>
@@ -8223,8 +8270,8 @@
       <c r="H119" s="14"/>
       <c r="I119" s="14"/>
       <c r="J119" s="15"/>
-      <c r="K119" s="23"/>
-      <c r="L119" s="24"/>
+      <c r="K119" s="27"/>
+      <c r="L119" s="28"/>
     </row>
     <row r="120" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A120" s="11"/>
@@ -8237,8 +8284,8 @@
       <c r="H120" s="14"/>
       <c r="I120" s="14"/>
       <c r="J120" s="15"/>
-      <c r="K120" s="23"/>
-      <c r="L120" s="24"/>
+      <c r="K120" s="27"/>
+      <c r="L120" s="28"/>
     </row>
     <row r="121" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A121" s="11"/>
@@ -8251,8 +8298,8 @@
       <c r="H121" s="14"/>
       <c r="I121" s="14"/>
       <c r="J121" s="15"/>
-      <c r="K121" s="23"/>
-      <c r="L121" s="24"/>
+      <c r="K121" s="27"/>
+      <c r="L121" s="28"/>
     </row>
     <row r="122" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A122" s="11"/>
@@ -8265,8 +8312,8 @@
       <c r="H122" s="14"/>
       <c r="I122" s="14"/>
       <c r="J122" s="15"/>
-      <c r="K122" s="23"/>
-      <c r="L122" s="24"/>
+      <c r="K122" s="27"/>
+      <c r="L122" s="28"/>
     </row>
     <row r="123" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A123" s="11"/>
@@ -8279,8 +8326,8 @@
       <c r="H123" s="14"/>
       <c r="I123" s="14"/>
       <c r="J123" s="15"/>
-      <c r="K123" s="23"/>
-      <c r="L123" s="24"/>
+      <c r="K123" s="27"/>
+      <c r="L123" s="28"/>
     </row>
     <row r="124" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A124" s="11"/>
@@ -8293,8 +8340,8 @@
       <c r="H124" s="14"/>
       <c r="I124" s="14"/>
       <c r="J124" s="15"/>
-      <c r="K124" s="23"/>
-      <c r="L124" s="24"/>
+      <c r="K124" s="27"/>
+      <c r="L124" s="28"/>
     </row>
     <row r="125" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A125" s="11"/>
@@ -8307,8 +8354,8 @@
       <c r="H125" s="14"/>
       <c r="I125" s="14"/>
       <c r="J125" s="15"/>
-      <c r="K125" s="23"/>
-      <c r="L125" s="24"/>
+      <c r="K125" s="27"/>
+      <c r="L125" s="28"/>
     </row>
     <row r="126" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A126" s="11"/>
@@ -8321,8 +8368,8 @@
       <c r="H126" s="14"/>
       <c r="I126" s="14"/>
       <c r="J126" s="15"/>
-      <c r="K126" s="23"/>
-      <c r="L126" s="24"/>
+      <c r="K126" s="27"/>
+      <c r="L126" s="28"/>
     </row>
     <row r="127" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A127" s="11"/>
@@ -8335,8 +8382,8 @@
       <c r="H127" s="14"/>
       <c r="I127" s="14"/>
       <c r="J127" s="15"/>
-      <c r="K127" s="23"/>
-      <c r="L127" s="24"/>
+      <c r="K127" s="27"/>
+      <c r="L127" s="28"/>
     </row>
     <row r="128" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A128" s="11"/>
@@ -8349,8 +8396,8 @@
       <c r="H128" s="14"/>
       <c r="I128" s="14"/>
       <c r="J128" s="15"/>
-      <c r="K128" s="23"/>
-      <c r="L128" s="24"/>
+      <c r="K128" s="27"/>
+      <c r="L128" s="28"/>
     </row>
     <row r="129" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A129" s="11"/>
@@ -8363,8 +8410,8 @@
       <c r="H129" s="14"/>
       <c r="I129" s="14"/>
       <c r="J129" s="15"/>
-      <c r="K129" s="23"/>
-      <c r="L129" s="24"/>
+      <c r="K129" s="27"/>
+      <c r="L129" s="28"/>
     </row>
     <row r="130" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A130" s="11"/>
@@ -8377,8 +8424,8 @@
       <c r="H130" s="14"/>
       <c r="I130" s="14"/>
       <c r="J130" s="15"/>
-      <c r="K130" s="23"/>
-      <c r="L130" s="24"/>
+      <c r="K130" s="27"/>
+      <c r="L130" s="28"/>
     </row>
     <row r="131" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A131" s="11"/>
@@ -8391,8 +8438,8 @@
       <c r="H131" s="14"/>
       <c r="I131" s="14"/>
       <c r="J131" s="15"/>
-      <c r="K131" s="23"/>
-      <c r="L131" s="24"/>
+      <c r="K131" s="27"/>
+      <c r="L131" s="28"/>
     </row>
     <row r="132" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A132" s="11"/>
@@ -8405,8 +8452,8 @@
       <c r="H132" s="14"/>
       <c r="I132" s="14"/>
       <c r="J132" s="15"/>
-      <c r="K132" s="23"/>
-      <c r="L132" s="24"/>
+      <c r="K132" s="27"/>
+      <c r="L132" s="28"/>
     </row>
     <row r="133" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A133" s="11"/>
@@ -8419,8 +8466,8 @@
       <c r="H133" s="14"/>
       <c r="I133" s="14"/>
       <c r="J133" s="15"/>
-      <c r="K133" s="23"/>
-      <c r="L133" s="24"/>
+      <c r="K133" s="27"/>
+      <c r="L133" s="28"/>
     </row>
     <row r="134" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A134" s="11"/>
@@ -8433,8 +8480,8 @@
       <c r="H134" s="14"/>
       <c r="I134" s="14"/>
       <c r="J134" s="15"/>
-      <c r="K134" s="23"/>
-      <c r="L134" s="24"/>
+      <c r="K134" s="27"/>
+      <c r="L134" s="28"/>
     </row>
     <row r="135" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A135" s="11"/>
@@ -8447,8 +8494,8 @@
       <c r="H135" s="14"/>
       <c r="I135" s="14"/>
       <c r="J135" s="15"/>
-      <c r="K135" s="23"/>
-      <c r="L135" s="24"/>
+      <c r="K135" s="27"/>
+      <c r="L135" s="28"/>
     </row>
     <row r="136" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A136" s="11"/>
@@ -8461,8 +8508,8 @@
       <c r="H136" s="14"/>
       <c r="I136" s="14"/>
       <c r="J136" s="15"/>
-      <c r="K136" s="23"/>
-      <c r="L136" s="24"/>
+      <c r="K136" s="27"/>
+      <c r="L136" s="28"/>
     </row>
     <row r="137" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A137" s="11"/>
@@ -8475,8 +8522,8 @@
       <c r="H137" s="14"/>
       <c r="I137" s="14"/>
       <c r="J137" s="15"/>
-      <c r="K137" s="23"/>
-      <c r="L137" s="24"/>
+      <c r="K137" s="27"/>
+      <c r="L137" s="28"/>
     </row>
     <row r="138" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A138" s="11"/>
@@ -8489,8 +8536,8 @@
       <c r="H138" s="14"/>
       <c r="I138" s="14"/>
       <c r="J138" s="15"/>
-      <c r="K138" s="23"/>
-      <c r="L138" s="24"/>
+      <c r="K138" s="27"/>
+      <c r="L138" s="28"/>
     </row>
     <row r="139" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A139" s="11"/>
@@ -8503,8 +8550,8 @@
       <c r="H139" s="14"/>
       <c r="I139" s="14"/>
       <c r="J139" s="15"/>
-      <c r="K139" s="23"/>
-      <c r="L139" s="24"/>
+      <c r="K139" s="27"/>
+      <c r="L139" s="28"/>
     </row>
     <row r="140" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A140" s="11"/>
@@ -8517,8 +8564,8 @@
       <c r="H140" s="14"/>
       <c r="I140" s="14"/>
       <c r="J140" s="15"/>
-      <c r="K140" s="23"/>
-      <c r="L140" s="24"/>
+      <c r="K140" s="27"/>
+      <c r="L140" s="28"/>
     </row>
     <row r="141" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A141" s="11"/>
@@ -8531,8 +8578,8 @@
       <c r="H141" s="14"/>
       <c r="I141" s="14"/>
       <c r="J141" s="15"/>
-      <c r="K141" s="23"/>
-      <c r="L141" s="24"/>
+      <c r="K141" s="27"/>
+      <c r="L141" s="28"/>
     </row>
     <row r="142" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A142" s="11"/>
@@ -8545,8 +8592,8 @@
       <c r="H142" s="14"/>
       <c r="I142" s="14"/>
       <c r="J142" s="15"/>
-      <c r="K142" s="23"/>
-      <c r="L142" s="24"/>
+      <c r="K142" s="27"/>
+      <c r="L142" s="28"/>
     </row>
     <row r="143" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A143" s="11"/>
@@ -8559,8 +8606,8 @@
       <c r="H143" s="14"/>
       <c r="I143" s="14"/>
       <c r="J143" s="15"/>
-      <c r="K143" s="23"/>
-      <c r="L143" s="24"/>
+      <c r="K143" s="27"/>
+      <c r="L143" s="28"/>
     </row>
     <row r="144" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A144" s="11"/>
@@ -8573,8 +8620,8 @@
       <c r="H144" s="14"/>
       <c r="I144" s="14"/>
       <c r="J144" s="15"/>
-      <c r="K144" s="23"/>
-      <c r="L144" s="24"/>
+      <c r="K144" s="27"/>
+      <c r="L144" s="28"/>
     </row>
     <row r="145" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A145" s="11"/>
@@ -8587,8 +8634,8 @@
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
       <c r="J145" s="15"/>
-      <c r="K145" s="23"/>
-      <c r="L145" s="24"/>
+      <c r="K145" s="27"/>
+      <c r="L145" s="28"/>
     </row>
     <row r="146" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A146" s="11"/>
@@ -8601,8 +8648,8 @@
       <c r="H146" s="14"/>
       <c r="I146" s="14"/>
       <c r="J146" s="15"/>
-      <c r="K146" s="23"/>
-      <c r="L146" s="24"/>
+      <c r="K146" s="27"/>
+      <c r="L146" s="28"/>
     </row>
     <row r="147" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A147" s="11"/>
@@ -8615,8 +8662,8 @@
       <c r="H147" s="14"/>
       <c r="I147" s="14"/>
       <c r="J147" s="15"/>
-      <c r="K147" s="23"/>
-      <c r="L147" s="24"/>
+      <c r="K147" s="27"/>
+      <c r="L147" s="28"/>
     </row>
     <row r="148" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A148" s="11"/>
@@ -8629,8 +8676,8 @@
       <c r="H148" s="14"/>
       <c r="I148" s="14"/>
       <c r="J148" s="15"/>
-      <c r="K148" s="23"/>
-      <c r="L148" s="24"/>
+      <c r="K148" s="27"/>
+      <c r="L148" s="28"/>
     </row>
     <row r="149" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A149" s="11"/>
@@ -8643,8 +8690,8 @@
       <c r="H149" s="14"/>
       <c r="I149" s="14"/>
       <c r="J149" s="15"/>
-      <c r="K149" s="23"/>
-      <c r="L149" s="24"/>
+      <c r="K149" s="27"/>
+      <c r="L149" s="28"/>
     </row>
     <row r="150" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A150" s="11"/>
@@ -8657,8 +8704,8 @@
       <c r="H150" s="14"/>
       <c r="I150" s="14"/>
       <c r="J150" s="15"/>
-      <c r="K150" s="23"/>
-      <c r="L150" s="24"/>
+      <c r="K150" s="27"/>
+      <c r="L150" s="28"/>
     </row>
     <row r="151" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A151" s="11"/>
@@ -8671,8 +8718,8 @@
       <c r="H151" s="14"/>
       <c r="I151" s="14"/>
       <c r="J151" s="15"/>
-      <c r="K151" s="23"/>
-      <c r="L151" s="24"/>
+      <c r="K151" s="27"/>
+      <c r="L151" s="28"/>
     </row>
     <row r="152" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A152" s="11"/>
@@ -8685,8 +8732,8 @@
       <c r="H152" s="14"/>
       <c r="I152" s="14"/>
       <c r="J152" s="15"/>
-      <c r="K152" s="23"/>
-      <c r="L152" s="24"/>
+      <c r="K152" s="27"/>
+      <c r="L152" s="28"/>
     </row>
     <row r="153" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A153" s="11"/>
@@ -8699,8 +8746,8 @@
       <c r="H153" s="14"/>
       <c r="I153" s="14"/>
       <c r="J153" s="15"/>
-      <c r="K153" s="23"/>
-      <c r="L153" s="24"/>
+      <c r="K153" s="27"/>
+      <c r="L153" s="28"/>
     </row>
     <row r="154" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A154" s="11"/>
@@ -8713,8 +8760,8 @@
       <c r="H154" s="14"/>
       <c r="I154" s="14"/>
       <c r="J154" s="15"/>
-      <c r="K154" s="23"/>
-      <c r="L154" s="24"/>
+      <c r="K154" s="27"/>
+      <c r="L154" s="28"/>
     </row>
     <row r="155" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A155" s="11"/>
@@ -8727,8 +8774,8 @@
       <c r="H155" s="14"/>
       <c r="I155" s="14"/>
       <c r="J155" s="15"/>
-      <c r="K155" s="23"/>
-      <c r="L155" s="24"/>
+      <c r="K155" s="27"/>
+      <c r="L155" s="28"/>
     </row>
     <row r="156" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A156" s="11"/>
@@ -8741,8 +8788,8 @@
       <c r="H156" s="14"/>
       <c r="I156" s="14"/>
       <c r="J156" s="15"/>
-      <c r="K156" s="23"/>
-      <c r="L156" s="24"/>
+      <c r="K156" s="27"/>
+      <c r="L156" s="28"/>
     </row>
     <row r="157" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A157" s="11"/>
@@ -8755,8 +8802,8 @@
       <c r="H157" s="14"/>
       <c r="I157" s="14"/>
       <c r="J157" s="15"/>
-      <c r="K157" s="23"/>
-      <c r="L157" s="24"/>
+      <c r="K157" s="27"/>
+      <c r="L157" s="28"/>
     </row>
     <row r="158" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A158" s="11"/>
@@ -8769,8 +8816,8 @@
       <c r="H158" s="14"/>
       <c r="I158" s="14"/>
       <c r="J158" s="15"/>
-      <c r="K158" s="23"/>
-      <c r="L158" s="24"/>
+      <c r="K158" s="27"/>
+      <c r="L158" s="28"/>
     </row>
     <row r="159" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A159" s="11"/>
@@ -8783,8 +8830,8 @@
       <c r="H159" s="14"/>
       <c r="I159" s="14"/>
       <c r="J159" s="15"/>
-      <c r="K159" s="23"/>
-      <c r="L159" s="24"/>
+      <c r="K159" s="27"/>
+      <c r="L159" s="28"/>
     </row>
     <row r="160" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A160" s="11"/>
@@ -8797,8 +8844,8 @@
       <c r="H160" s="14"/>
       <c r="I160" s="14"/>
       <c r="J160" s="15"/>
-      <c r="K160" s="23"/>
-      <c r="L160" s="24"/>
+      <c r="K160" s="27"/>
+      <c r="L160" s="28"/>
     </row>
     <row r="161" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A161" s="11"/>
@@ -8811,8 +8858,8 @@
       <c r="H161" s="14"/>
       <c r="I161" s="14"/>
       <c r="J161" s="15"/>
-      <c r="K161" s="23"/>
-      <c r="L161" s="24"/>
+      <c r="K161" s="27"/>
+      <c r="L161" s="28"/>
     </row>
     <row r="162" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A162" s="11"/>
@@ -8825,8 +8872,8 @@
       <c r="H162" s="14"/>
       <c r="I162" s="14"/>
       <c r="J162" s="15"/>
-      <c r="K162" s="23"/>
-      <c r="L162" s="24"/>
+      <c r="K162" s="27"/>
+      <c r="L162" s="28"/>
     </row>
     <row r="163" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A163" s="11"/>
@@ -8839,8 +8886,8 @@
       <c r="H163" s="14"/>
       <c r="I163" s="14"/>
       <c r="J163" s="15"/>
-      <c r="K163" s="23"/>
-      <c r="L163" s="24"/>
+      <c r="K163" s="27"/>
+      <c r="L163" s="28"/>
     </row>
     <row r="164" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A164" s="11"/>
@@ -8853,8 +8900,8 @@
       <c r="H164" s="14"/>
       <c r="I164" s="14"/>
       <c r="J164" s="15"/>
-      <c r="K164" s="23"/>
-      <c r="L164" s="24"/>
+      <c r="K164" s="27"/>
+      <c r="L164" s="28"/>
     </row>
     <row r="165" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A165" s="11"/>
@@ -8867,8 +8914,8 @@
       <c r="H165" s="14"/>
       <c r="I165" s="14"/>
       <c r="J165" s="15"/>
-      <c r="K165" s="23"/>
-      <c r="L165" s="24"/>
+      <c r="K165" s="27"/>
+      <c r="L165" s="28"/>
     </row>
     <row r="166" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A166" s="11"/>
@@ -8881,8 +8928,8 @@
       <c r="H166" s="14"/>
       <c r="I166" s="14"/>
       <c r="J166" s="15"/>
-      <c r="K166" s="23"/>
-      <c r="L166" s="24"/>
+      <c r="K166" s="27"/>
+      <c r="L166" s="28"/>
     </row>
     <row r="167" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A167" s="11"/>
@@ -8895,8 +8942,8 @@
       <c r="H167" s="14"/>
       <c r="I167" s="14"/>
       <c r="J167" s="15"/>
-      <c r="K167" s="23"/>
-      <c r="L167" s="24"/>
+      <c r="K167" s="27"/>
+      <c r="L167" s="28"/>
     </row>
     <row r="168" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A168" s="11"/>
@@ -8909,8 +8956,8 @@
       <c r="H168" s="14"/>
       <c r="I168" s="14"/>
       <c r="J168" s="15"/>
-      <c r="K168" s="23"/>
-      <c r="L168" s="24"/>
+      <c r="K168" s="27"/>
+      <c r="L168" s="28"/>
     </row>
     <row r="169" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A169" s="11"/>
@@ -8923,8 +8970,8 @@
       <c r="H169" s="14"/>
       <c r="I169" s="14"/>
       <c r="J169" s="15"/>
-      <c r="K169" s="23"/>
-      <c r="L169" s="24"/>
+      <c r="K169" s="27"/>
+      <c r="L169" s="28"/>
     </row>
     <row r="170" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A170" s="11"/>
@@ -8937,8 +8984,8 @@
       <c r="H170" s="14"/>
       <c r="I170" s="14"/>
       <c r="J170" s="15"/>
-      <c r="K170" s="23"/>
-      <c r="L170" s="24"/>
+      <c r="K170" s="27"/>
+      <c r="L170" s="28"/>
     </row>
     <row r="171" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A171" s="11"/>
@@ -8951,8 +8998,8 @@
       <c r="H171" s="14"/>
       <c r="I171" s="14"/>
       <c r="J171" s="15"/>
-      <c r="K171" s="23"/>
-      <c r="L171" s="24"/>
+      <c r="K171" s="27"/>
+      <c r="L171" s="28"/>
     </row>
     <row r="172" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A172" s="11"/>
@@ -8965,8 +9012,8 @@
       <c r="H172" s="14"/>
       <c r="I172" s="14"/>
       <c r="J172" s="15"/>
-      <c r="K172" s="23"/>
-      <c r="L172" s="24"/>
+      <c r="K172" s="27"/>
+      <c r="L172" s="28"/>
     </row>
     <row r="173" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A173" s="11"/>
@@ -8979,8 +9026,8 @@
       <c r="H173" s="14"/>
       <c r="I173" s="14"/>
       <c r="J173" s="15"/>
-      <c r="K173" s="23"/>
-      <c r="L173" s="24"/>
+      <c r="K173" s="27"/>
+      <c r="L173" s="28"/>
     </row>
     <row r="174" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A174" s="11"/>
@@ -8993,8 +9040,8 @@
       <c r="H174" s="14"/>
       <c r="I174" s="14"/>
       <c r="J174" s="15"/>
-      <c r="K174" s="23"/>
-      <c r="L174" s="24"/>
+      <c r="K174" s="27"/>
+      <c r="L174" s="28"/>
     </row>
     <row r="175" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A175" s="11"/>
@@ -9007,8 +9054,8 @@
       <c r="H175" s="14"/>
       <c r="I175" s="14"/>
       <c r="J175" s="15"/>
-      <c r="K175" s="23"/>
-      <c r="L175" s="24"/>
+      <c r="K175" s="27"/>
+      <c r="L175" s="28"/>
     </row>
     <row r="176" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A176" s="11"/>
@@ -9021,8 +9068,8 @@
       <c r="H176" s="14"/>
       <c r="I176" s="14"/>
       <c r="J176" s="15"/>
-      <c r="K176" s="23"/>
-      <c r="L176" s="24"/>
+      <c r="K176" s="27"/>
+      <c r="L176" s="28"/>
     </row>
     <row r="177" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A177" s="11"/>
@@ -9035,8 +9082,8 @@
       <c r="H177" s="14"/>
       <c r="I177" s="14"/>
       <c r="J177" s="15"/>
-      <c r="K177" s="23"/>
-      <c r="L177" s="24"/>
+      <c r="K177" s="27"/>
+      <c r="L177" s="28"/>
     </row>
     <row r="178" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A178" s="11"/>
@@ -9049,8 +9096,8 @@
       <c r="H178" s="14"/>
       <c r="I178" s="14"/>
       <c r="J178" s="15"/>
-      <c r="K178" s="23"/>
-      <c r="L178" s="24"/>
+      <c r="K178" s="27"/>
+      <c r="L178" s="28"/>
     </row>
     <row r="179" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A179" s="11"/>
@@ -9063,8 +9110,8 @@
       <c r="H179" s="14"/>
       <c r="I179" s="14"/>
       <c r="J179" s="15"/>
-      <c r="K179" s="23"/>
-      <c r="L179" s="24"/>
+      <c r="K179" s="27"/>
+      <c r="L179" s="28"/>
     </row>
     <row r="180" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A180" s="11"/>
@@ -9077,8 +9124,8 @@
       <c r="H180" s="14"/>
       <c r="I180" s="14"/>
       <c r="J180" s="15"/>
-      <c r="K180" s="23"/>
-      <c r="L180" s="24"/>
+      <c r="K180" s="27"/>
+      <c r="L180" s="28"/>
     </row>
     <row r="181" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A181" s="11"/>
@@ -9091,8 +9138,8 @@
       <c r="H181" s="14"/>
       <c r="I181" s="14"/>
       <c r="J181" s="15"/>
-      <c r="K181" s="23"/>
-      <c r="L181" s="24"/>
+      <c r="K181" s="27"/>
+      <c r="L181" s="28"/>
     </row>
     <row r="182" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A182" s="11"/>
@@ -9105,8 +9152,8 @@
       <c r="H182" s="14"/>
       <c r="I182" s="14"/>
       <c r="J182" s="15"/>
-      <c r="K182" s="23"/>
-      <c r="L182" s="24"/>
+      <c r="K182" s="27"/>
+      <c r="L182" s="28"/>
     </row>
     <row r="183" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A183" s="11"/>
@@ -9119,8 +9166,8 @@
       <c r="H183" s="14"/>
       <c r="I183" s="14"/>
       <c r="J183" s="15"/>
-      <c r="K183" s="23"/>
-      <c r="L183" s="24"/>
+      <c r="K183" s="27"/>
+      <c r="L183" s="28"/>
     </row>
     <row r="184" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A184" s="11"/>
@@ -9133,8 +9180,8 @@
       <c r="H184" s="14"/>
       <c r="I184" s="14"/>
       <c r="J184" s="15"/>
-      <c r="K184" s="23"/>
-      <c r="L184" s="24"/>
+      <c r="K184" s="27"/>
+      <c r="L184" s="28"/>
     </row>
     <row r="185" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A185" s="11"/>
@@ -9147,8 +9194,8 @@
       <c r="H185" s="14"/>
       <c r="I185" s="14"/>
       <c r="J185" s="15"/>
-      <c r="K185" s="23"/>
-      <c r="L185" s="24"/>
+      <c r="K185" s="27"/>
+      <c r="L185" s="28"/>
     </row>
     <row r="186" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A186" s="11"/>
@@ -9161,8 +9208,8 @@
       <c r="H186" s="14"/>
       <c r="I186" s="14"/>
       <c r="J186" s="15"/>
-      <c r="K186" s="23"/>
-      <c r="L186" s="24"/>
+      <c r="K186" s="27"/>
+      <c r="L186" s="28"/>
     </row>
     <row r="187" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A187" s="11"/>
@@ -9175,8 +9222,8 @@
       <c r="H187" s="14"/>
       <c r="I187" s="14"/>
       <c r="J187" s="15"/>
-      <c r="K187" s="23"/>
-      <c r="L187" s="24"/>
+      <c r="K187" s="27"/>
+      <c r="L187" s="28"/>
     </row>
     <row r="188" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A188" s="11"/>
@@ -9189,8 +9236,8 @@
       <c r="H188" s="14"/>
       <c r="I188" s="14"/>
       <c r="J188" s="15"/>
-      <c r="K188" s="23"/>
-      <c r="L188" s="24"/>
+      <c r="K188" s="27"/>
+      <c r="L188" s="28"/>
     </row>
     <row r="189" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A189" s="11"/>
@@ -9203,8 +9250,8 @@
       <c r="H189" s="14"/>
       <c r="I189" s="14"/>
       <c r="J189" s="15"/>
-      <c r="K189" s="23"/>
-      <c r="L189" s="24"/>
+      <c r="K189" s="27"/>
+      <c r="L189" s="28"/>
     </row>
     <row r="190" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A190" s="11"/>
@@ -9217,8 +9264,8 @@
       <c r="H190" s="14"/>
       <c r="I190" s="14"/>
       <c r="J190" s="15"/>
-      <c r="K190" s="23"/>
-      <c r="L190" s="24"/>
+      <c r="K190" s="27"/>
+      <c r="L190" s="28"/>
     </row>
     <row r="191" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A191" s="11"/>
@@ -9231,8 +9278,8 @@
       <c r="H191" s="14"/>
       <c r="I191" s="14"/>
       <c r="J191" s="15"/>
-      <c r="K191" s="23"/>
-      <c r="L191" s="24"/>
+      <c r="K191" s="27"/>
+      <c r="L191" s="28"/>
     </row>
     <row r="192" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A192" s="11"/>
@@ -9245,45 +9292,59 @@
       <c r="H192" s="14"/>
       <c r="I192" s="14"/>
       <c r="J192" s="15"/>
-      <c r="K192" s="23"/>
-      <c r="L192" s="24"/>
+      <c r="K192" s="27"/>
+      <c r="L192" s="28"/>
+    </row>
+    <row r="193" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
+      <c r="A193" s="11"/>
+      <c r="B193" s="12"/>
+      <c r="C193" s="13"/>
+      <c r="D193" s="14"/>
+      <c r="E193" s="14"/>
+      <c r="F193" s="14"/>
+      <c r="G193" s="14"/>
+      <c r="H193" s="14"/>
+      <c r="I193" s="14"/>
+      <c r="J193" s="15"/>
+      <c r="K193" s="27"/>
+      <c r="L193" s="28"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
-  <conditionalFormatting sqref="N20">
+  <conditionalFormatting sqref="N21">
     <cfRule type="beginsWith" dxfId="0" priority="13" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N20,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N21,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="14" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N20,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N21,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="15" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N20,LEN("PASS"))="PASS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N23">
-    <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N23,LEN("WARN"))="WARN"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N23,LEN("FAIL"))="FAIL"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="9" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N23,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N21,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N24">
-    <cfRule type="beginsWith" dxfId="0" priority="16" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N24,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N24,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="9" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N24,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16:N19">
+  <conditionalFormatting sqref="N25">
+    <cfRule type="beginsWith" dxfId="0" priority="16" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N25,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N25,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N25,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16:N20">
     <cfRule type="beginsWith" dxfId="0" priority="22" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N16,LEN("WARN"))="WARN"</formula>
     </cfRule>
@@ -9294,22 +9355,22 @@
       <formula>LEFT(N16,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N21:N22">
+  <conditionalFormatting sqref="N22:N23">
     <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="equal" text="WARN">
-      <formula>LEFT(N21,LEN("WARN"))="WARN"</formula>
+      <formula>LEFT(N22,LEN("WARN"))="WARN"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="FAIL">
-      <formula>LEFT(N21,LEN("FAIL"))="FAIL"</formula>
+      <formula>LEFT(N22,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
     <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="PASS">
-      <formula>LEFT(N21,LEN("PASS"))="PASS"</formula>
+      <formula>LEFT(N22,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D5 D6 D9 D10 D11 D12 D13 D14 D15 D18 D19 D20 D21 D22 D23 D24 D25 D2:D3 D7:D8 D16:D17 D26:D192">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D5 D6 D9 D10 D11 D12 D13 D14 D15 D18 D19 D20 D21 D22 D23 D24 D25 D26 D2:D3 D7:D8 D16:D17 D27:D193">
       <formula1>INDIRECT(C2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C11 C12 C13 C14 C15 C18 C19 C20 C21 C22 C23 C24 C25 C2:C3 C4:C5 C7:C8 C9:C10 C16:C17 C26:C192">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C11 C12 C13 C14 C15 C18 C19 C20 C21 C22 C23 C24 C25 C26 C2:C3 C4:C5 C7:C8 C9:C10 C16:C17 C27:C193">
       <formula1>target</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Mobile UI - Purchase and Sale Order
</commit_message>
<xml_diff>
--- a/tests/artifact/script/GNUKhata.macro.xlsx
+++ b/tests/artifact/script/GNUKhata.macro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="788">
   <si>
     <t>target</t>
   </si>
@@ -2456,41 +2456,62 @@
     <t>${input.username}</t>
   </si>
   <si>
+    <t>${login.username}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    And I type the Password</t>
+  </si>
+  <si>
+    <t>${input.password}</t>
+  </si>
+  <si>
+    <t>${login.password}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    And I click on the submit button</t>
+  </si>
+  <si>
+    <t>${button.submit}</t>
+  </si>
+  <si>
+    <t>user should be navigated to GNU Dashboard</t>
+  </si>
+  <si>
+    <t>${title.locator}</t>
+  </si>
+  <si>
+    <t>${title.header}</t>
+  </si>
+  <si>
+    <t>mobilelogin</t>
+  </si>
+  <si>
+    <t>Resize the window for mobile testing</t>
+  </si>
+  <si>
+    <t>wait for login page to load</t>
+  </si>
+  <si>
     <t>${username}</t>
   </si>
   <si>
-    <t xml:space="preserve">    And I type the Password</t>
-  </si>
-  <si>
-    <t>${input.password}</t>
-  </si>
-  <si>
     <t>${password}</t>
   </si>
   <si>
-    <t xml:space="preserve">    And I click on the submit button</t>
-  </si>
-  <si>
-    <t>${button.submit}</t>
-  </si>
-  <si>
-    <t>user should be navigated to GNU Dashboard</t>
-  </si>
-  <si>
-    <t>${title.header}</t>
+    <t>Welcome Accion!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2525,34 +2546,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-0.0499893185216834"/>
       <name val="Tahoma"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -2563,18 +2561,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2587,6 +2601,37 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2594,15 +2639,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2616,55 +2662,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2679,6 +2678,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2705,7 +2718,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2717,7 +2730,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2729,7 +2748,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2741,19 +2856,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2765,127 +2898,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2915,16 +2928,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2944,37 +2975,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3005,16 +3016,24 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3023,143 +3042,137 @@
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3215,23 +3228,11 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3250,52 +3251,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -3617,7 +3618,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="18" width="8.33333333333333" customWidth="1" collapsed="1"/>
   </cols>
@@ -6287,13 +6288,13 @@
   <sheetPr/>
   <dimension ref="A1:O192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="$A24:$XFD24"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20.1666666666667" style="3" customWidth="1"/>
     <col min="2" max="2" width="31.5" style="4" customWidth="1"/>
@@ -6337,15 +6338,15 @@
       <c r="I1" s="10" t="s">
         <v>731</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="18" t="s">
         <v>732</v>
       </c>
-      <c r="K1" s="22"/>
+      <c r="K1" s="19"/>
       <c r="L1" s="10" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="41.4" spans="1:12">
+    <row r="2" s="2" customFormat="1" ht="42" spans="1:12">
       <c r="A2" s="11" t="s">
         <v>734</v>
       </c>
@@ -6368,8 +6369,8 @@
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="15"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="24"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="3" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A3" s="11"/>
@@ -6390,8 +6391,8 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="4" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A4" s="11"/>
@@ -6414,8 +6415,8 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="15"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
     </row>
     <row r="5" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A5" s="11"/>
@@ -6436,10 +6437,10 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="24"/>
-    </row>
-    <row r="6" s="2" customFormat="1" ht="41.4" spans="1:12">
+      <c r="K5" s="20"/>
+      <c r="L5" s="21"/>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="42" spans="1:12">
       <c r="A6" s="11" t="s">
         <v>744</v>
       </c>
@@ -6462,8 +6463,8 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="18" customHeight="1" spans="3:12">
       <c r="C7" s="13" t="s">
@@ -6482,8 +6483,8 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="15"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="24"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="21"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A8" s="11"/>
@@ -6504,8 +6505,8 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="15"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A9" s="11"/>
@@ -6528,8 +6529,8 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="15"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="21"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A10" s="11"/>
@@ -6550,10 +6551,10 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="15"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="24"/>
-    </row>
-    <row r="11" s="2" customFormat="1" ht="96.6" spans="1:12">
+      <c r="K10" s="20"/>
+      <c r="L10" s="21"/>
+    </row>
+    <row r="11" s="2" customFormat="1" ht="98" spans="1:12">
       <c r="A11" s="11" t="s">
         <v>750</v>
       </c>
@@ -6576,8 +6577,8 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="15"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="24"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="21"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A12" s="11"/>
@@ -6598,8 +6599,8 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="15"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="24"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="21"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A13" s="11"/>
@@ -6620,8 +6621,8 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="15"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="24"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="21"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A14" s="11"/>
@@ -6644,8 +6645,8 @@
       <c r="J14" s="15" t="s">
         <v>760</v>
       </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="21"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A15" s="11"/>
@@ -6664,10 +6665,10 @@
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="27.6" spans="1:15">
+      <c r="K15" s="20"/>
+      <c r="L15" s="21"/>
+    </row>
+    <row r="16" s="2" customFormat="1" ht="28" spans="1:15">
       <c r="A16" s="11" t="s">
         <v>762</v>
       </c>
@@ -6690,11 +6691,11 @@
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="23"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="20"/>
     </row>
     <row r="17" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A17" s="11"/>
@@ -6711,11 +6712,11 @@
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="23"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="20"/>
     </row>
     <row r="18" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A18" s="11"/>
@@ -6736,11 +6737,11 @@
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="15"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="23"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="20"/>
     </row>
     <row r="19" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A19" s="11"/>
@@ -6761,11 +6762,11 @@
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="15"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="23"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="20"/>
     </row>
     <row r="20" s="2" customFormat="1" ht="22" customHeight="1" spans="1:15">
       <c r="A20" s="11"/>
@@ -6786,11 +6787,11 @@
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="15"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="23"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="20"/>
     </row>
     <row r="21" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A21" s="11"/>
@@ -6813,11 +6814,11 @@
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="15"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="23"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="20"/>
     </row>
     <row r="22" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A22" s="11"/>
@@ -6840,11 +6841,11 @@
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="15"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="23"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="20"/>
     </row>
     <row r="23" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A23" s="11"/>
@@ -6865,11 +6866,11 @@
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="15"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="25"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="23"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="20"/>
     </row>
     <row r="24" s="2" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A24" s="11"/>
@@ -6880,147 +6881,262 @@
         <v>30</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>559</v>
+        <v>535</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>780</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="14" t="s">
+        <v>781</v>
+      </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="23"/>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="20"/>
+    </row>
+    <row r="25" s="2" customFormat="1" ht="28" spans="1:15">
+      <c r="A25" s="11" t="s">
+        <v>782</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>763</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>764</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>765</v>
+      </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="15"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="24"/>
-    </row>
-    <row r="26" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K25" s="20"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="20"/>
+    </row>
+    <row r="26" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="B26" s="12" t="s">
+        <v>783</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>640</v>
+      </c>
+      <c r="E26" s="2">
+        <v>430</v>
+      </c>
+      <c r="F26" s="2">
+        <v>932</v>
+      </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="24"/>
-    </row>
-    <row r="27" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K26" s="20"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="20"/>
+    </row>
+    <row r="27" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A27" s="11"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="B27" s="12" t="s">
+        <v>784</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>767</v>
+      </c>
+      <c r="F27" s="17">
+        <v>5000</v>
+      </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="15"/>
-      <c r="K27" s="23"/>
-      <c r="L27" s="24"/>
-    </row>
-    <row r="28" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K27" s="20"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="20"/>
+    </row>
+    <row r="28" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="B28" s="12" t="s">
+        <v>768</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>767</v>
+      </c>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="15"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="24"/>
-    </row>
-    <row r="29" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K28" s="20"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="20"/>
+    </row>
+    <row r="29" s="2" customFormat="1" ht="22" customHeight="1" spans="1:15">
       <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
+      <c r="B29" s="12" t="s">
+        <v>769</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>713</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>770</v>
+      </c>
+      <c r="F29" s="15"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="15"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="24"/>
-    </row>
-    <row r="30" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K29" s="20"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="22"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="20"/>
+    </row>
+    <row r="30" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
+      <c r="B30" s="12" t="s">
+        <v>771</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>772</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>785</v>
+      </c>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="15"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="24"/>
-    </row>
-    <row r="31" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K30" s="20"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="20"/>
+    </row>
+    <row r="31" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="14"/>
+      <c r="B31" s="12" t="s">
+        <v>774</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>705</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>775</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>786</v>
+      </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="15"/>
-      <c r="K31" s="23"/>
-      <c r="L31" s="24"/>
-    </row>
-    <row r="32" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K31" s="20"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="22"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="20"/>
+    </row>
+    <row r="32" s="2" customFormat="1" ht="23" customHeight="1" spans="1:15">
       <c r="A32" s="11"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="B32" s="12" t="s">
+        <v>777</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>778</v>
+      </c>
       <c r="F32" s="14"/>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="15"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="24"/>
-    </row>
-    <row r="33" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
+      <c r="K32" s="20"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="20"/>
+    </row>
+    <row r="33" s="2" customFormat="1" ht="19" customHeight="1" spans="1:15">
       <c r="A33" s="11"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="B33" s="12" t="s">
+        <v>779</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>780</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>787</v>
+      </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="15"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="24"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="20"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A34" s="11"/>
@@ -7033,8 +7149,8 @@
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="15"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="24"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="21"/>
     </row>
     <row r="35" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A35" s="11"/>
@@ -7047,8 +7163,8 @@
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="15"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="24"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="21"/>
     </row>
     <row r="36" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A36" s="11"/>
@@ -7061,8 +7177,8 @@
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="15"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="24"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="21"/>
     </row>
     <row r="37" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A37" s="11"/>
@@ -7075,8 +7191,8 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="15"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="24"/>
+      <c r="K37" s="20"/>
+      <c r="L37" s="21"/>
     </row>
     <row r="38" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A38" s="11"/>
@@ -7089,8 +7205,8 @@
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="15"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="24"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="21"/>
     </row>
     <row r="39" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A39" s="11"/>
@@ -7103,8 +7219,8 @@
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="15"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="24"/>
+      <c r="K39" s="20"/>
+      <c r="L39" s="21"/>
     </row>
     <row r="40" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A40" s="11"/>
@@ -7117,8 +7233,8 @@
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="15"/>
-      <c r="K40" s="23"/>
-      <c r="L40" s="24"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="21"/>
     </row>
     <row r="41" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A41" s="11"/>
@@ -7131,8 +7247,8 @@
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="15"/>
-      <c r="K41" s="23"/>
-      <c r="L41" s="24"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="21"/>
     </row>
     <row r="42" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A42" s="11"/>
@@ -7145,8 +7261,8 @@
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="15"/>
-      <c r="K42" s="23"/>
-      <c r="L42" s="24"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="21"/>
     </row>
     <row r="43" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A43" s="11"/>
@@ -7159,8 +7275,8 @@
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="15"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="24"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="21"/>
     </row>
     <row r="44" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A44" s="11"/>
@@ -7173,8 +7289,8 @@
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="15"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="24"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="21"/>
     </row>
     <row r="45" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A45" s="11"/>
@@ -7187,8 +7303,8 @@
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="15"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="24"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="21"/>
     </row>
     <row r="46" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A46" s="11"/>
@@ -7201,8 +7317,8 @@
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="15"/>
-      <c r="K46" s="23"/>
-      <c r="L46" s="24"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="21"/>
     </row>
     <row r="47" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A47" s="11"/>
@@ -7215,8 +7331,8 @@
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="15"/>
-      <c r="K47" s="23"/>
-      <c r="L47" s="24"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="21"/>
     </row>
     <row r="48" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A48" s="11"/>
@@ -7229,8 +7345,8 @@
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="15"/>
-      <c r="K48" s="23"/>
-      <c r="L48" s="24"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="21"/>
     </row>
     <row r="49" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A49" s="11"/>
@@ -7243,8 +7359,8 @@
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
       <c r="J49" s="15"/>
-      <c r="K49" s="23"/>
-      <c r="L49" s="24"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="21"/>
     </row>
     <row r="50" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A50" s="11"/>
@@ -7257,8 +7373,8 @@
       <c r="H50" s="14"/>
       <c r="I50" s="14"/>
       <c r="J50" s="15"/>
-      <c r="K50" s="23"/>
-      <c r="L50" s="24"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="21"/>
     </row>
     <row r="51" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A51" s="11"/>
@@ -7271,8 +7387,8 @@
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
       <c r="J51" s="15"/>
-      <c r="K51" s="23"/>
-      <c r="L51" s="24"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="21"/>
     </row>
     <row r="52" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A52" s="11"/>
@@ -7285,8 +7401,8 @@
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
       <c r="J52" s="15"/>
-      <c r="K52" s="23"/>
-      <c r="L52" s="24"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="21"/>
     </row>
     <row r="53" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A53" s="11"/>
@@ -7299,8 +7415,8 @@
       <c r="H53" s="14"/>
       <c r="I53" s="14"/>
       <c r="J53" s="15"/>
-      <c r="K53" s="23"/>
-      <c r="L53" s="24"/>
+      <c r="K53" s="20"/>
+      <c r="L53" s="21"/>
     </row>
     <row r="54" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A54" s="11"/>
@@ -7313,8 +7429,8 @@
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
       <c r="J54" s="15"/>
-      <c r="K54" s="23"/>
-      <c r="L54" s="24"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="21"/>
     </row>
     <row r="55" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A55" s="11"/>
@@ -7327,8 +7443,8 @@
       <c r="H55" s="14"/>
       <c r="I55" s="14"/>
       <c r="J55" s="15"/>
-      <c r="K55" s="23"/>
-      <c r="L55" s="24"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="21"/>
     </row>
     <row r="56" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A56" s="11"/>
@@ -7341,8 +7457,8 @@
       <c r="H56" s="14"/>
       <c r="I56" s="14"/>
       <c r="J56" s="15"/>
-      <c r="K56" s="23"/>
-      <c r="L56" s="24"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="21"/>
     </row>
     <row r="57" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A57" s="11"/>
@@ -7355,8 +7471,8 @@
       <c r="H57" s="14"/>
       <c r="I57" s="14"/>
       <c r="J57" s="15"/>
-      <c r="K57" s="23"/>
-      <c r="L57" s="24"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="21"/>
     </row>
     <row r="58" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A58" s="11"/>
@@ -7369,8 +7485,8 @@
       <c r="H58" s="14"/>
       <c r="I58" s="14"/>
       <c r="J58" s="15"/>
-      <c r="K58" s="23"/>
-      <c r="L58" s="24"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="21"/>
     </row>
     <row r="59" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A59" s="11"/>
@@ -7383,8 +7499,8 @@
       <c r="H59" s="14"/>
       <c r="I59" s="14"/>
       <c r="J59" s="15"/>
-      <c r="K59" s="23"/>
-      <c r="L59" s="24"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="21"/>
     </row>
     <row r="60" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A60" s="11"/>
@@ -7397,8 +7513,8 @@
       <c r="H60" s="14"/>
       <c r="I60" s="14"/>
       <c r="J60" s="15"/>
-      <c r="K60" s="23"/>
-      <c r="L60" s="24"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="21"/>
     </row>
     <row r="61" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A61" s="11"/>
@@ -7411,8 +7527,8 @@
       <c r="H61" s="14"/>
       <c r="I61" s="14"/>
       <c r="J61" s="15"/>
-      <c r="K61" s="23"/>
-      <c r="L61" s="24"/>
+      <c r="K61" s="20"/>
+      <c r="L61" s="21"/>
     </row>
     <row r="62" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A62" s="11"/>
@@ -7425,8 +7541,8 @@
       <c r="H62" s="14"/>
       <c r="I62" s="14"/>
       <c r="J62" s="15"/>
-      <c r="K62" s="23"/>
-      <c r="L62" s="24"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="21"/>
     </row>
     <row r="63" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A63" s="11"/>
@@ -7439,8 +7555,8 @@
       <c r="H63" s="14"/>
       <c r="I63" s="14"/>
       <c r="J63" s="15"/>
-      <c r="K63" s="23"/>
-      <c r="L63" s="24"/>
+      <c r="K63" s="20"/>
+      <c r="L63" s="21"/>
     </row>
     <row r="64" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A64" s="11"/>
@@ -7453,8 +7569,8 @@
       <c r="H64" s="14"/>
       <c r="I64" s="14"/>
       <c r="J64" s="15"/>
-      <c r="K64" s="23"/>
-      <c r="L64" s="24"/>
+      <c r="K64" s="20"/>
+      <c r="L64" s="21"/>
     </row>
     <row r="65" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A65" s="11"/>
@@ -7467,8 +7583,8 @@
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
       <c r="J65" s="15"/>
-      <c r="K65" s="23"/>
-      <c r="L65" s="24"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="21"/>
     </row>
     <row r="66" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A66" s="11"/>
@@ -7481,8 +7597,8 @@
       <c r="H66" s="14"/>
       <c r="I66" s="14"/>
       <c r="J66" s="15"/>
-      <c r="K66" s="23"/>
-      <c r="L66" s="24"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="21"/>
     </row>
     <row r="67" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A67" s="11"/>
@@ -7495,8 +7611,8 @@
       <c r="H67" s="14"/>
       <c r="I67" s="14"/>
       <c r="J67" s="15"/>
-      <c r="K67" s="23"/>
-      <c r="L67" s="24"/>
+      <c r="K67" s="20"/>
+      <c r="L67" s="21"/>
     </row>
     <row r="68" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A68" s="11"/>
@@ -7509,8 +7625,8 @@
       <c r="H68" s="14"/>
       <c r="I68" s="14"/>
       <c r="J68" s="15"/>
-      <c r="K68" s="23"/>
-      <c r="L68" s="24"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="21"/>
     </row>
     <row r="69" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A69" s="11"/>
@@ -7523,8 +7639,8 @@
       <c r="H69" s="14"/>
       <c r="I69" s="14"/>
       <c r="J69" s="15"/>
-      <c r="K69" s="23"/>
-      <c r="L69" s="24"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="21"/>
     </row>
     <row r="70" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A70" s="11"/>
@@ -7537,8 +7653,8 @@
       <c r="H70" s="14"/>
       <c r="I70" s="14"/>
       <c r="J70" s="15"/>
-      <c r="K70" s="23"/>
-      <c r="L70" s="24"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="21"/>
     </row>
     <row r="71" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A71" s="11"/>
@@ -7551,8 +7667,8 @@
       <c r="H71" s="14"/>
       <c r="I71" s="14"/>
       <c r="J71" s="15"/>
-      <c r="K71" s="23"/>
-      <c r="L71" s="24"/>
+      <c r="K71" s="20"/>
+      <c r="L71" s="21"/>
     </row>
     <row r="72" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A72" s="11"/>
@@ -7565,8 +7681,8 @@
       <c r="H72" s="14"/>
       <c r="I72" s="14"/>
       <c r="J72" s="15"/>
-      <c r="K72" s="23"/>
-      <c r="L72" s="24"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="21"/>
     </row>
     <row r="73" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A73" s="11"/>
@@ -7579,8 +7695,8 @@
       <c r="H73" s="14"/>
       <c r="I73" s="14"/>
       <c r="J73" s="15"/>
-      <c r="K73" s="23"/>
-      <c r="L73" s="24"/>
+      <c r="K73" s="20"/>
+      <c r="L73" s="21"/>
     </row>
     <row r="74" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A74" s="11"/>
@@ -7593,8 +7709,8 @@
       <c r="H74" s="14"/>
       <c r="I74" s="14"/>
       <c r="J74" s="15"/>
-      <c r="K74" s="23"/>
-      <c r="L74" s="24"/>
+      <c r="K74" s="20"/>
+      <c r="L74" s="21"/>
     </row>
     <row r="75" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A75" s="11"/>
@@ -7607,8 +7723,8 @@
       <c r="H75" s="14"/>
       <c r="I75" s="14"/>
       <c r="J75" s="15"/>
-      <c r="K75" s="23"/>
-      <c r="L75" s="24"/>
+      <c r="K75" s="20"/>
+      <c r="L75" s="21"/>
     </row>
     <row r="76" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A76" s="11"/>
@@ -7621,8 +7737,8 @@
       <c r="H76" s="14"/>
       <c r="I76" s="14"/>
       <c r="J76" s="15"/>
-      <c r="K76" s="23"/>
-      <c r="L76" s="24"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="21"/>
     </row>
     <row r="77" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A77" s="11"/>
@@ -7635,8 +7751,8 @@
       <c r="H77" s="14"/>
       <c r="I77" s="14"/>
       <c r="J77" s="15"/>
-      <c r="K77" s="23"/>
-      <c r="L77" s="24"/>
+      <c r="K77" s="20"/>
+      <c r="L77" s="21"/>
     </row>
     <row r="78" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A78" s="11"/>
@@ -7649,8 +7765,8 @@
       <c r="H78" s="14"/>
       <c r="I78" s="14"/>
       <c r="J78" s="15"/>
-      <c r="K78" s="23"/>
-      <c r="L78" s="24"/>
+      <c r="K78" s="20"/>
+      <c r="L78" s="21"/>
     </row>
     <row r="79" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A79" s="11"/>
@@ -7663,8 +7779,8 @@
       <c r="H79" s="14"/>
       <c r="I79" s="14"/>
       <c r="J79" s="15"/>
-      <c r="K79" s="23"/>
-      <c r="L79" s="24"/>
+      <c r="K79" s="20"/>
+      <c r="L79" s="21"/>
     </row>
     <row r="80" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A80" s="11"/>
@@ -7677,8 +7793,8 @@
       <c r="H80" s="14"/>
       <c r="I80" s="14"/>
       <c r="J80" s="15"/>
-      <c r="K80" s="23"/>
-      <c r="L80" s="24"/>
+      <c r="K80" s="20"/>
+      <c r="L80" s="21"/>
     </row>
     <row r="81" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A81" s="11"/>
@@ -7691,8 +7807,8 @@
       <c r="H81" s="14"/>
       <c r="I81" s="14"/>
       <c r="J81" s="15"/>
-      <c r="K81" s="23"/>
-      <c r="L81" s="24"/>
+      <c r="K81" s="20"/>
+      <c r="L81" s="21"/>
     </row>
     <row r="82" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A82" s="11"/>
@@ -7705,8 +7821,8 @@
       <c r="H82" s="14"/>
       <c r="I82" s="14"/>
       <c r="J82" s="15"/>
-      <c r="K82" s="23"/>
-      <c r="L82" s="24"/>
+      <c r="K82" s="20"/>
+      <c r="L82" s="21"/>
     </row>
     <row r="83" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A83" s="11"/>
@@ -7719,8 +7835,8 @@
       <c r="H83" s="14"/>
       <c r="I83" s="14"/>
       <c r="J83" s="15"/>
-      <c r="K83" s="23"/>
-      <c r="L83" s="24"/>
+      <c r="K83" s="20"/>
+      <c r="L83" s="21"/>
     </row>
     <row r="84" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A84" s="11"/>
@@ -7733,8 +7849,8 @@
       <c r="H84" s="14"/>
       <c r="I84" s="14"/>
       <c r="J84" s="15"/>
-      <c r="K84" s="23"/>
-      <c r="L84" s="24"/>
+      <c r="K84" s="20"/>
+      <c r="L84" s="21"/>
     </row>
     <row r="85" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A85" s="11"/>
@@ -7747,8 +7863,8 @@
       <c r="H85" s="14"/>
       <c r="I85" s="14"/>
       <c r="J85" s="15"/>
-      <c r="K85" s="23"/>
-      <c r="L85" s="24"/>
+      <c r="K85" s="20"/>
+      <c r="L85" s="21"/>
     </row>
     <row r="86" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A86" s="11"/>
@@ -7761,8 +7877,8 @@
       <c r="H86" s="14"/>
       <c r="I86" s="14"/>
       <c r="J86" s="15"/>
-      <c r="K86" s="23"/>
-      <c r="L86" s="24"/>
+      <c r="K86" s="20"/>
+      <c r="L86" s="21"/>
     </row>
     <row r="87" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A87" s="11"/>
@@ -7775,8 +7891,8 @@
       <c r="H87" s="14"/>
       <c r="I87" s="14"/>
       <c r="J87" s="15"/>
-      <c r="K87" s="23"/>
-      <c r="L87" s="24"/>
+      <c r="K87" s="20"/>
+      <c r="L87" s="21"/>
     </row>
     <row r="88" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A88" s="11"/>
@@ -7789,8 +7905,8 @@
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
       <c r="J88" s="15"/>
-      <c r="K88" s="23"/>
-      <c r="L88" s="24"/>
+      <c r="K88" s="20"/>
+      <c r="L88" s="21"/>
     </row>
     <row r="89" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A89" s="11"/>
@@ -7803,8 +7919,8 @@
       <c r="H89" s="14"/>
       <c r="I89" s="14"/>
       <c r="J89" s="15"/>
-      <c r="K89" s="23"/>
-      <c r="L89" s="24"/>
+      <c r="K89" s="20"/>
+      <c r="L89" s="21"/>
     </row>
     <row r="90" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A90" s="11"/>
@@ -7817,8 +7933,8 @@
       <c r="H90" s="14"/>
       <c r="I90" s="14"/>
       <c r="J90" s="15"/>
-      <c r="K90" s="23"/>
-      <c r="L90" s="24"/>
+      <c r="K90" s="20"/>
+      <c r="L90" s="21"/>
     </row>
     <row r="91" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A91" s="11"/>
@@ -7831,8 +7947,8 @@
       <c r="H91" s="14"/>
       <c r="I91" s="14"/>
       <c r="J91" s="15"/>
-      <c r="K91" s="23"/>
-      <c r="L91" s="24"/>
+      <c r="K91" s="20"/>
+      <c r="L91" s="21"/>
     </row>
     <row r="92" s="2" customFormat="1" ht="23" customHeight="1" spans="1:12">
       <c r="A92" s="11"/>
@@ -7845,8 +7961,8 @@
       <c r="H92" s="14"/>
       <c r="I92" s="14"/>
       <c r="J92" s="15"/>
-      <c r="K92" s="23"/>
-      <c r="L92" s="24"/>
+      <c r="K92" s="20"/>
+      <c r="L92" s="21"/>
     </row>
     <row r="93" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A93" s="11"/>
@@ -7859,8 +7975,8 @@
       <c r="H93" s="14"/>
       <c r="I93" s="14"/>
       <c r="J93" s="15"/>
-      <c r="K93" s="23"/>
-      <c r="L93" s="24"/>
+      <c r="K93" s="20"/>
+      <c r="L93" s="21"/>
     </row>
     <row r="94" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A94" s="11"/>
@@ -7873,8 +7989,8 @@
       <c r="H94" s="14"/>
       <c r="I94" s="14"/>
       <c r="J94" s="15"/>
-      <c r="K94" s="23"/>
-      <c r="L94" s="24"/>
+      <c r="K94" s="20"/>
+      <c r="L94" s="21"/>
     </row>
     <row r="95" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A95" s="11"/>
@@ -7887,8 +8003,8 @@
       <c r="H95" s="14"/>
       <c r="I95" s="14"/>
       <c r="J95" s="15"/>
-      <c r="K95" s="23"/>
-      <c r="L95" s="24"/>
+      <c r="K95" s="20"/>
+      <c r="L95" s="21"/>
     </row>
     <row r="96" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A96" s="11"/>
@@ -7901,8 +8017,8 @@
       <c r="H96" s="14"/>
       <c r="I96" s="14"/>
       <c r="J96" s="15"/>
-      <c r="K96" s="23"/>
-      <c r="L96" s="24"/>
+      <c r="K96" s="20"/>
+      <c r="L96" s="21"/>
     </row>
     <row r="97" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A97" s="11"/>
@@ -7915,8 +8031,8 @@
       <c r="H97" s="14"/>
       <c r="I97" s="14"/>
       <c r="J97" s="15"/>
-      <c r="K97" s="23"/>
-      <c r="L97" s="24"/>
+      <c r="K97" s="20"/>
+      <c r="L97" s="21"/>
     </row>
     <row r="98" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A98" s="11"/>
@@ -7929,8 +8045,8 @@
       <c r="H98" s="14"/>
       <c r="I98" s="14"/>
       <c r="J98" s="15"/>
-      <c r="K98" s="23"/>
-      <c r="L98" s="24"/>
+      <c r="K98" s="20"/>
+      <c r="L98" s="21"/>
     </row>
     <row r="99" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A99" s="11"/>
@@ -7943,8 +8059,8 @@
       <c r="H99" s="14"/>
       <c r="I99" s="14"/>
       <c r="J99" s="15"/>
-      <c r="K99" s="23"/>
-      <c r="L99" s="24"/>
+      <c r="K99" s="20"/>
+      <c r="L99" s="21"/>
     </row>
     <row r="100" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A100" s="11"/>
@@ -7957,8 +8073,8 @@
       <c r="H100" s="14"/>
       <c r="I100" s="14"/>
       <c r="J100" s="15"/>
-      <c r="K100" s="23"/>
-      <c r="L100" s="24"/>
+      <c r="K100" s="20"/>
+      <c r="L100" s="21"/>
     </row>
     <row r="101" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A101" s="11"/>
@@ -7971,8 +8087,8 @@
       <c r="H101" s="14"/>
       <c r="I101" s="14"/>
       <c r="J101" s="15"/>
-      <c r="K101" s="23"/>
-      <c r="L101" s="24"/>
+      <c r="K101" s="20"/>
+      <c r="L101" s="21"/>
     </row>
     <row r="102" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A102" s="11"/>
@@ -7985,8 +8101,8 @@
       <c r="H102" s="14"/>
       <c r="I102" s="14"/>
       <c r="J102" s="15"/>
-      <c r="K102" s="23"/>
-      <c r="L102" s="24"/>
+      <c r="K102" s="20"/>
+      <c r="L102" s="21"/>
     </row>
     <row r="103" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A103" s="11"/>
@@ -7999,8 +8115,8 @@
       <c r="H103" s="14"/>
       <c r="I103" s="14"/>
       <c r="J103" s="15"/>
-      <c r="K103" s="23"/>
-      <c r="L103" s="24"/>
+      <c r="K103" s="20"/>
+      <c r="L103" s="21"/>
     </row>
     <row r="104" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A104" s="11"/>
@@ -8013,8 +8129,8 @@
       <c r="H104" s="14"/>
       <c r="I104" s="14"/>
       <c r="J104" s="15"/>
-      <c r="K104" s="23"/>
-      <c r="L104" s="24"/>
+      <c r="K104" s="20"/>
+      <c r="L104" s="21"/>
     </row>
     <row r="105" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A105" s="11"/>
@@ -8027,8 +8143,8 @@
       <c r="H105" s="14"/>
       <c r="I105" s="14"/>
       <c r="J105" s="15"/>
-      <c r="K105" s="23"/>
-      <c r="L105" s="24"/>
+      <c r="K105" s="20"/>
+      <c r="L105" s="21"/>
     </row>
     <row r="106" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A106" s="11"/>
@@ -8041,8 +8157,8 @@
       <c r="H106" s="14"/>
       <c r="I106" s="14"/>
       <c r="J106" s="15"/>
-      <c r="K106" s="23"/>
-      <c r="L106" s="24"/>
+      <c r="K106" s="20"/>
+      <c r="L106" s="21"/>
     </row>
     <row r="107" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A107" s="11"/>
@@ -8055,8 +8171,8 @@
       <c r="H107" s="14"/>
       <c r="I107" s="14"/>
       <c r="J107" s="15"/>
-      <c r="K107" s="23"/>
-      <c r="L107" s="24"/>
+      <c r="K107" s="20"/>
+      <c r="L107" s="21"/>
     </row>
     <row r="108" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A108" s="11"/>
@@ -8069,8 +8185,8 @@
       <c r="H108" s="14"/>
       <c r="I108" s="14"/>
       <c r="J108" s="15"/>
-      <c r="K108" s="23"/>
-      <c r="L108" s="24"/>
+      <c r="K108" s="20"/>
+      <c r="L108" s="21"/>
     </row>
     <row r="109" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A109" s="11"/>
@@ -8083,8 +8199,8 @@
       <c r="H109" s="14"/>
       <c r="I109" s="14"/>
       <c r="J109" s="15"/>
-      <c r="K109" s="23"/>
-      <c r="L109" s="24"/>
+      <c r="K109" s="20"/>
+      <c r="L109" s="21"/>
     </row>
     <row r="110" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A110" s="11"/>
@@ -8097,8 +8213,8 @@
       <c r="H110" s="14"/>
       <c r="I110" s="14"/>
       <c r="J110" s="15"/>
-      <c r="K110" s="23"/>
-      <c r="L110" s="24"/>
+      <c r="K110" s="20"/>
+      <c r="L110" s="21"/>
     </row>
     <row r="111" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A111" s="11"/>
@@ -8111,8 +8227,8 @@
       <c r="H111" s="14"/>
       <c r="I111" s="14"/>
       <c r="J111" s="15"/>
-      <c r="K111" s="23"/>
-      <c r="L111" s="24"/>
+      <c r="K111" s="20"/>
+      <c r="L111" s="21"/>
     </row>
     <row r="112" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A112" s="11"/>
@@ -8125,8 +8241,8 @@
       <c r="H112" s="14"/>
       <c r="I112" s="14"/>
       <c r="J112" s="15"/>
-      <c r="K112" s="23"/>
-      <c r="L112" s="24"/>
+      <c r="K112" s="20"/>
+      <c r="L112" s="21"/>
     </row>
     <row r="113" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A113" s="11"/>
@@ -8139,8 +8255,8 @@
       <c r="H113" s="14"/>
       <c r="I113" s="14"/>
       <c r="J113" s="15"/>
-      <c r="K113" s="23"/>
-      <c r="L113" s="24"/>
+      <c r="K113" s="20"/>
+      <c r="L113" s="21"/>
     </row>
     <row r="114" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A114" s="11"/>
@@ -8153,8 +8269,8 @@
       <c r="H114" s="14"/>
       <c r="I114" s="14"/>
       <c r="J114" s="15"/>
-      <c r="K114" s="23"/>
-      <c r="L114" s="24"/>
+      <c r="K114" s="20"/>
+      <c r="L114" s="21"/>
     </row>
     <row r="115" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A115" s="11"/>
@@ -8167,8 +8283,8 @@
       <c r="H115" s="14"/>
       <c r="I115" s="14"/>
       <c r="J115" s="15"/>
-      <c r="K115" s="23"/>
-      <c r="L115" s="24"/>
+      <c r="K115" s="20"/>
+      <c r="L115" s="21"/>
     </row>
     <row r="116" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A116" s="11"/>
@@ -8181,8 +8297,8 @@
       <c r="H116" s="14"/>
       <c r="I116" s="14"/>
       <c r="J116" s="15"/>
-      <c r="K116" s="23"/>
-      <c r="L116" s="24"/>
+      <c r="K116" s="20"/>
+      <c r="L116" s="21"/>
     </row>
     <row r="117" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A117" s="11"/>
@@ -8195,8 +8311,8 @@
       <c r="H117" s="14"/>
       <c r="I117" s="14"/>
       <c r="J117" s="15"/>
-      <c r="K117" s="23"/>
-      <c r="L117" s="24"/>
+      <c r="K117" s="20"/>
+      <c r="L117" s="21"/>
     </row>
     <row r="118" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A118" s="11"/>
@@ -8209,8 +8325,8 @@
       <c r="H118" s="14"/>
       <c r="I118" s="14"/>
       <c r="J118" s="15"/>
-      <c r="K118" s="23"/>
-      <c r="L118" s="24"/>
+      <c r="K118" s="20"/>
+      <c r="L118" s="21"/>
     </row>
     <row r="119" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A119" s="11"/>
@@ -8223,8 +8339,8 @@
       <c r="H119" s="14"/>
       <c r="I119" s="14"/>
       <c r="J119" s="15"/>
-      <c r="K119" s="23"/>
-      <c r="L119" s="24"/>
+      <c r="K119" s="20"/>
+      <c r="L119" s="21"/>
     </row>
     <row r="120" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A120" s="11"/>
@@ -8237,8 +8353,8 @@
       <c r="H120" s="14"/>
       <c r="I120" s="14"/>
       <c r="J120" s="15"/>
-      <c r="K120" s="23"/>
-      <c r="L120" s="24"/>
+      <c r="K120" s="20"/>
+      <c r="L120" s="21"/>
     </row>
     <row r="121" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A121" s="11"/>
@@ -8251,8 +8367,8 @@
       <c r="H121" s="14"/>
       <c r="I121" s="14"/>
       <c r="J121" s="15"/>
-      <c r="K121" s="23"/>
-      <c r="L121" s="24"/>
+      <c r="K121" s="20"/>
+      <c r="L121" s="21"/>
     </row>
     <row r="122" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A122" s="11"/>
@@ -8265,8 +8381,8 @@
       <c r="H122" s="14"/>
       <c r="I122" s="14"/>
       <c r="J122" s="15"/>
-      <c r="K122" s="23"/>
-      <c r="L122" s="24"/>
+      <c r="K122" s="20"/>
+      <c r="L122" s="21"/>
     </row>
     <row r="123" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A123" s="11"/>
@@ -8279,8 +8395,8 @@
       <c r="H123" s="14"/>
       <c r="I123" s="14"/>
       <c r="J123" s="15"/>
-      <c r="K123" s="23"/>
-      <c r="L123" s="24"/>
+      <c r="K123" s="20"/>
+      <c r="L123" s="21"/>
     </row>
     <row r="124" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A124" s="11"/>
@@ -8293,8 +8409,8 @@
       <c r="H124" s="14"/>
       <c r="I124" s="14"/>
       <c r="J124" s="15"/>
-      <c r="K124" s="23"/>
-      <c r="L124" s="24"/>
+      <c r="K124" s="20"/>
+      <c r="L124" s="21"/>
     </row>
     <row r="125" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A125" s="11"/>
@@ -8307,8 +8423,8 @@
       <c r="H125" s="14"/>
       <c r="I125" s="14"/>
       <c r="J125" s="15"/>
-      <c r="K125" s="23"/>
-      <c r="L125" s="24"/>
+      <c r="K125" s="20"/>
+      <c r="L125" s="21"/>
     </row>
     <row r="126" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A126" s="11"/>
@@ -8321,8 +8437,8 @@
       <c r="H126" s="14"/>
       <c r="I126" s="14"/>
       <c r="J126" s="15"/>
-      <c r="K126" s="23"/>
-      <c r="L126" s="24"/>
+      <c r="K126" s="20"/>
+      <c r="L126" s="21"/>
     </row>
     <row r="127" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A127" s="11"/>
@@ -8335,8 +8451,8 @@
       <c r="H127" s="14"/>
       <c r="I127" s="14"/>
       <c r="J127" s="15"/>
-      <c r="K127" s="23"/>
-      <c r="L127" s="24"/>
+      <c r="K127" s="20"/>
+      <c r="L127" s="21"/>
     </row>
     <row r="128" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A128" s="11"/>
@@ -8349,8 +8465,8 @@
       <c r="H128" s="14"/>
       <c r="I128" s="14"/>
       <c r="J128" s="15"/>
-      <c r="K128" s="23"/>
-      <c r="L128" s="24"/>
+      <c r="K128" s="20"/>
+      <c r="L128" s="21"/>
     </row>
     <row r="129" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A129" s="11"/>
@@ -8363,8 +8479,8 @@
       <c r="H129" s="14"/>
       <c r="I129" s="14"/>
       <c r="J129" s="15"/>
-      <c r="K129" s="23"/>
-      <c r="L129" s="24"/>
+      <c r="K129" s="20"/>
+      <c r="L129" s="21"/>
     </row>
     <row r="130" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A130" s="11"/>
@@ -8377,8 +8493,8 @@
       <c r="H130" s="14"/>
       <c r="I130" s="14"/>
       <c r="J130" s="15"/>
-      <c r="K130" s="23"/>
-      <c r="L130" s="24"/>
+      <c r="K130" s="20"/>
+      <c r="L130" s="21"/>
     </row>
     <row r="131" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A131" s="11"/>
@@ -8391,8 +8507,8 @@
       <c r="H131" s="14"/>
       <c r="I131" s="14"/>
       <c r="J131" s="15"/>
-      <c r="K131" s="23"/>
-      <c r="L131" s="24"/>
+      <c r="K131" s="20"/>
+      <c r="L131" s="21"/>
     </row>
     <row r="132" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A132" s="11"/>
@@ -8405,8 +8521,8 @@
       <c r="H132" s="14"/>
       <c r="I132" s="14"/>
       <c r="J132" s="15"/>
-      <c r="K132" s="23"/>
-      <c r="L132" s="24"/>
+      <c r="K132" s="20"/>
+      <c r="L132" s="21"/>
     </row>
     <row r="133" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A133" s="11"/>
@@ -8419,8 +8535,8 @@
       <c r="H133" s="14"/>
       <c r="I133" s="14"/>
       <c r="J133" s="15"/>
-      <c r="K133" s="23"/>
-      <c r="L133" s="24"/>
+      <c r="K133" s="20"/>
+      <c r="L133" s="21"/>
     </row>
     <row r="134" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A134" s="11"/>
@@ -8433,8 +8549,8 @@
       <c r="H134" s="14"/>
       <c r="I134" s="14"/>
       <c r="J134" s="15"/>
-      <c r="K134" s="23"/>
-      <c r="L134" s="24"/>
+      <c r="K134" s="20"/>
+      <c r="L134" s="21"/>
     </row>
     <row r="135" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A135" s="11"/>
@@ -8447,8 +8563,8 @@
       <c r="H135" s="14"/>
       <c r="I135" s="14"/>
       <c r="J135" s="15"/>
-      <c r="K135" s="23"/>
-      <c r="L135" s="24"/>
+      <c r="K135" s="20"/>
+      <c r="L135" s="21"/>
     </row>
     <row r="136" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A136" s="11"/>
@@ -8461,8 +8577,8 @@
       <c r="H136" s="14"/>
       <c r="I136" s="14"/>
       <c r="J136" s="15"/>
-      <c r="K136" s="23"/>
-      <c r="L136" s="24"/>
+      <c r="K136" s="20"/>
+      <c r="L136" s="21"/>
     </row>
     <row r="137" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A137" s="11"/>
@@ -8475,8 +8591,8 @@
       <c r="H137" s="14"/>
       <c r="I137" s="14"/>
       <c r="J137" s="15"/>
-      <c r="K137" s="23"/>
-      <c r="L137" s="24"/>
+      <c r="K137" s="20"/>
+      <c r="L137" s="21"/>
     </row>
     <row r="138" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A138" s="11"/>
@@ -8489,8 +8605,8 @@
       <c r="H138" s="14"/>
       <c r="I138" s="14"/>
       <c r="J138" s="15"/>
-      <c r="K138" s="23"/>
-      <c r="L138" s="24"/>
+      <c r="K138" s="20"/>
+      <c r="L138" s="21"/>
     </row>
     <row r="139" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A139" s="11"/>
@@ -8503,8 +8619,8 @@
       <c r="H139" s="14"/>
       <c r="I139" s="14"/>
       <c r="J139" s="15"/>
-      <c r="K139" s="23"/>
-      <c r="L139" s="24"/>
+      <c r="K139" s="20"/>
+      <c r="L139" s="21"/>
     </row>
     <row r="140" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A140" s="11"/>
@@ -8517,8 +8633,8 @@
       <c r="H140" s="14"/>
       <c r="I140" s="14"/>
       <c r="J140" s="15"/>
-      <c r="K140" s="23"/>
-      <c r="L140" s="24"/>
+      <c r="K140" s="20"/>
+      <c r="L140" s="21"/>
     </row>
     <row r="141" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A141" s="11"/>
@@ -8531,8 +8647,8 @@
       <c r="H141" s="14"/>
       <c r="I141" s="14"/>
       <c r="J141" s="15"/>
-      <c r="K141" s="23"/>
-      <c r="L141" s="24"/>
+      <c r="K141" s="20"/>
+      <c r="L141" s="21"/>
     </row>
     <row r="142" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A142" s="11"/>
@@ -8545,8 +8661,8 @@
       <c r="H142" s="14"/>
       <c r="I142" s="14"/>
       <c r="J142" s="15"/>
-      <c r="K142" s="23"/>
-      <c r="L142" s="24"/>
+      <c r="K142" s="20"/>
+      <c r="L142" s="21"/>
     </row>
     <row r="143" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A143" s="11"/>
@@ -8559,8 +8675,8 @@
       <c r="H143" s="14"/>
       <c r="I143" s="14"/>
       <c r="J143" s="15"/>
-      <c r="K143" s="23"/>
-      <c r="L143" s="24"/>
+      <c r="K143" s="20"/>
+      <c r="L143" s="21"/>
     </row>
     <row r="144" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A144" s="11"/>
@@ -8573,8 +8689,8 @@
       <c r="H144" s="14"/>
       <c r="I144" s="14"/>
       <c r="J144" s="15"/>
-      <c r="K144" s="23"/>
-      <c r="L144" s="24"/>
+      <c r="K144" s="20"/>
+      <c r="L144" s="21"/>
     </row>
     <row r="145" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A145" s="11"/>
@@ -8587,8 +8703,8 @@
       <c r="H145" s="14"/>
       <c r="I145" s="14"/>
       <c r="J145" s="15"/>
-      <c r="K145" s="23"/>
-      <c r="L145" s="24"/>
+      <c r="K145" s="20"/>
+      <c r="L145" s="21"/>
     </row>
     <row r="146" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A146" s="11"/>
@@ -8601,8 +8717,8 @@
       <c r="H146" s="14"/>
       <c r="I146" s="14"/>
       <c r="J146" s="15"/>
-      <c r="K146" s="23"/>
-      <c r="L146" s="24"/>
+      <c r="K146" s="20"/>
+      <c r="L146" s="21"/>
     </row>
     <row r="147" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A147" s="11"/>
@@ -8615,8 +8731,8 @@
       <c r="H147" s="14"/>
       <c r="I147" s="14"/>
       <c r="J147" s="15"/>
-      <c r="K147" s="23"/>
-      <c r="L147" s="24"/>
+      <c r="K147" s="20"/>
+      <c r="L147" s="21"/>
     </row>
     <row r="148" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A148" s="11"/>
@@ -8629,8 +8745,8 @@
       <c r="H148" s="14"/>
       <c r="I148" s="14"/>
       <c r="J148" s="15"/>
-      <c r="K148" s="23"/>
-      <c r="L148" s="24"/>
+      <c r="K148" s="20"/>
+      <c r="L148" s="21"/>
     </row>
     <row r="149" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A149" s="11"/>
@@ -8643,8 +8759,8 @@
       <c r="H149" s="14"/>
       <c r="I149" s="14"/>
       <c r="J149" s="15"/>
-      <c r="K149" s="23"/>
-      <c r="L149" s="24"/>
+      <c r="K149" s="20"/>
+      <c r="L149" s="21"/>
     </row>
     <row r="150" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A150" s="11"/>
@@ -8657,8 +8773,8 @@
       <c r="H150" s="14"/>
       <c r="I150" s="14"/>
       <c r="J150" s="15"/>
-      <c r="K150" s="23"/>
-      <c r="L150" s="24"/>
+      <c r="K150" s="20"/>
+      <c r="L150" s="21"/>
     </row>
     <row r="151" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A151" s="11"/>
@@ -8671,8 +8787,8 @@
       <c r="H151" s="14"/>
       <c r="I151" s="14"/>
       <c r="J151" s="15"/>
-      <c r="K151" s="23"/>
-      <c r="L151" s="24"/>
+      <c r="K151" s="20"/>
+      <c r="L151" s="21"/>
     </row>
     <row r="152" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A152" s="11"/>
@@ -8685,8 +8801,8 @@
       <c r="H152" s="14"/>
       <c r="I152" s="14"/>
       <c r="J152" s="15"/>
-      <c r="K152" s="23"/>
-      <c r="L152" s="24"/>
+      <c r="K152" s="20"/>
+      <c r="L152" s="21"/>
     </row>
     <row r="153" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A153" s="11"/>
@@ -8699,8 +8815,8 @@
       <c r="H153" s="14"/>
       <c r="I153" s="14"/>
       <c r="J153" s="15"/>
-      <c r="K153" s="23"/>
-      <c r="L153" s="24"/>
+      <c r="K153" s="20"/>
+      <c r="L153" s="21"/>
     </row>
     <row r="154" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A154" s="11"/>
@@ -8713,8 +8829,8 @@
       <c r="H154" s="14"/>
       <c r="I154" s="14"/>
       <c r="J154" s="15"/>
-      <c r="K154" s="23"/>
-      <c r="L154" s="24"/>
+      <c r="K154" s="20"/>
+      <c r="L154" s="21"/>
     </row>
     <row r="155" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A155" s="11"/>
@@ -8727,8 +8843,8 @@
       <c r="H155" s="14"/>
       <c r="I155" s="14"/>
       <c r="J155" s="15"/>
-      <c r="K155" s="23"/>
-      <c r="L155" s="24"/>
+      <c r="K155" s="20"/>
+      <c r="L155" s="21"/>
     </row>
     <row r="156" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A156" s="11"/>
@@ -8741,8 +8857,8 @@
       <c r="H156" s="14"/>
       <c r="I156" s="14"/>
       <c r="J156" s="15"/>
-      <c r="K156" s="23"/>
-      <c r="L156" s="24"/>
+      <c r="K156" s="20"/>
+      <c r="L156" s="21"/>
     </row>
     <row r="157" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A157" s="11"/>
@@ -8755,8 +8871,8 @@
       <c r="H157" s="14"/>
       <c r="I157" s="14"/>
       <c r="J157" s="15"/>
-      <c r="K157" s="23"/>
-      <c r="L157" s="24"/>
+      <c r="K157" s="20"/>
+      <c r="L157" s="21"/>
     </row>
     <row r="158" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A158" s="11"/>
@@ -8769,8 +8885,8 @@
       <c r="H158" s="14"/>
       <c r="I158" s="14"/>
       <c r="J158" s="15"/>
-      <c r="K158" s="23"/>
-      <c r="L158" s="24"/>
+      <c r="K158" s="20"/>
+      <c r="L158" s="21"/>
     </row>
     <row r="159" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A159" s="11"/>
@@ -8783,8 +8899,8 @@
       <c r="H159" s="14"/>
       <c r="I159" s="14"/>
       <c r="J159" s="15"/>
-      <c r="K159" s="23"/>
-      <c r="L159" s="24"/>
+      <c r="K159" s="20"/>
+      <c r="L159" s="21"/>
     </row>
     <row r="160" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A160" s="11"/>
@@ -8797,8 +8913,8 @@
       <c r="H160" s="14"/>
       <c r="I160" s="14"/>
       <c r="J160" s="15"/>
-      <c r="K160" s="23"/>
-      <c r="L160" s="24"/>
+      <c r="K160" s="20"/>
+      <c r="L160" s="21"/>
     </row>
     <row r="161" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A161" s="11"/>
@@ -8811,8 +8927,8 @@
       <c r="H161" s="14"/>
       <c r="I161" s="14"/>
       <c r="J161" s="15"/>
-      <c r="K161" s="23"/>
-      <c r="L161" s="24"/>
+      <c r="K161" s="20"/>
+      <c r="L161" s="21"/>
     </row>
     <row r="162" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A162" s="11"/>
@@ -8825,8 +8941,8 @@
       <c r="H162" s="14"/>
       <c r="I162" s="14"/>
       <c r="J162" s="15"/>
-      <c r="K162" s="23"/>
-      <c r="L162" s="24"/>
+      <c r="K162" s="20"/>
+      <c r="L162" s="21"/>
     </row>
     <row r="163" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A163" s="11"/>
@@ -8839,8 +8955,8 @@
       <c r="H163" s="14"/>
       <c r="I163" s="14"/>
       <c r="J163" s="15"/>
-      <c r="K163" s="23"/>
-      <c r="L163" s="24"/>
+      <c r="K163" s="20"/>
+      <c r="L163" s="21"/>
     </row>
     <row r="164" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A164" s="11"/>
@@ -8853,8 +8969,8 @@
       <c r="H164" s="14"/>
       <c r="I164" s="14"/>
       <c r="J164" s="15"/>
-      <c r="K164" s="23"/>
-      <c r="L164" s="24"/>
+      <c r="K164" s="20"/>
+      <c r="L164" s="21"/>
     </row>
     <row r="165" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A165" s="11"/>
@@ -8867,8 +8983,8 @@
       <c r="H165" s="14"/>
       <c r="I165" s="14"/>
       <c r="J165" s="15"/>
-      <c r="K165" s="23"/>
-      <c r="L165" s="24"/>
+      <c r="K165" s="20"/>
+      <c r="L165" s="21"/>
     </row>
     <row r="166" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A166" s="11"/>
@@ -8881,8 +8997,8 @@
       <c r="H166" s="14"/>
       <c r="I166" s="14"/>
       <c r="J166" s="15"/>
-      <c r="K166" s="23"/>
-      <c r="L166" s="24"/>
+      <c r="K166" s="20"/>
+      <c r="L166" s="21"/>
     </row>
     <row r="167" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A167" s="11"/>
@@ -8895,8 +9011,8 @@
       <c r="H167" s="14"/>
       <c r="I167" s="14"/>
       <c r="J167" s="15"/>
-      <c r="K167" s="23"/>
-      <c r="L167" s="24"/>
+      <c r="K167" s="20"/>
+      <c r="L167" s="21"/>
     </row>
     <row r="168" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A168" s="11"/>
@@ -8909,8 +9025,8 @@
       <c r="H168" s="14"/>
       <c r="I168" s="14"/>
       <c r="J168" s="15"/>
-      <c r="K168" s="23"/>
-      <c r="L168" s="24"/>
+      <c r="K168" s="20"/>
+      <c r="L168" s="21"/>
     </row>
     <row r="169" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A169" s="11"/>
@@ -8923,8 +9039,8 @@
       <c r="H169" s="14"/>
       <c r="I169" s="14"/>
       <c r="J169" s="15"/>
-      <c r="K169" s="23"/>
-      <c r="L169" s="24"/>
+      <c r="K169" s="20"/>
+      <c r="L169" s="21"/>
     </row>
     <row r="170" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A170" s="11"/>
@@ -8937,8 +9053,8 @@
       <c r="H170" s="14"/>
       <c r="I170" s="14"/>
       <c r="J170" s="15"/>
-      <c r="K170" s="23"/>
-      <c r="L170" s="24"/>
+      <c r="K170" s="20"/>
+      <c r="L170" s="21"/>
     </row>
     <row r="171" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A171" s="11"/>
@@ -8951,8 +9067,8 @@
       <c r="H171" s="14"/>
       <c r="I171" s="14"/>
       <c r="J171" s="15"/>
-      <c r="K171" s="23"/>
-      <c r="L171" s="24"/>
+      <c r="K171" s="20"/>
+      <c r="L171" s="21"/>
     </row>
     <row r="172" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A172" s="11"/>
@@ -8965,8 +9081,8 @@
       <c r="H172" s="14"/>
       <c r="I172" s="14"/>
       <c r="J172" s="15"/>
-      <c r="K172" s="23"/>
-      <c r="L172" s="24"/>
+      <c r="K172" s="20"/>
+      <c r="L172" s="21"/>
     </row>
     <row r="173" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A173" s="11"/>
@@ -8979,8 +9095,8 @@
       <c r="H173" s="14"/>
       <c r="I173" s="14"/>
       <c r="J173" s="15"/>
-      <c r="K173" s="23"/>
-      <c r="L173" s="24"/>
+      <c r="K173" s="20"/>
+      <c r="L173" s="21"/>
     </row>
     <row r="174" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A174" s="11"/>
@@ -8993,8 +9109,8 @@
       <c r="H174" s="14"/>
       <c r="I174" s="14"/>
       <c r="J174" s="15"/>
-      <c r="K174" s="23"/>
-      <c r="L174" s="24"/>
+      <c r="K174" s="20"/>
+      <c r="L174" s="21"/>
     </row>
     <row r="175" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A175" s="11"/>
@@ -9007,8 +9123,8 @@
       <c r="H175" s="14"/>
       <c r="I175" s="14"/>
       <c r="J175" s="15"/>
-      <c r="K175" s="23"/>
-      <c r="L175" s="24"/>
+      <c r="K175" s="20"/>
+      <c r="L175" s="21"/>
     </row>
     <row r="176" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A176" s="11"/>
@@ -9021,8 +9137,8 @@
       <c r="H176" s="14"/>
       <c r="I176" s="14"/>
       <c r="J176" s="15"/>
-      <c r="K176" s="23"/>
-      <c r="L176" s="24"/>
+      <c r="K176" s="20"/>
+      <c r="L176" s="21"/>
     </row>
     <row r="177" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A177" s="11"/>
@@ -9035,8 +9151,8 @@
       <c r="H177" s="14"/>
       <c r="I177" s="14"/>
       <c r="J177" s="15"/>
-      <c r="K177" s="23"/>
-      <c r="L177" s="24"/>
+      <c r="K177" s="20"/>
+      <c r="L177" s="21"/>
     </row>
     <row r="178" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A178" s="11"/>
@@ -9049,8 +9165,8 @@
       <c r="H178" s="14"/>
       <c r="I178" s="14"/>
       <c r="J178" s="15"/>
-      <c r="K178" s="23"/>
-      <c r="L178" s="24"/>
+      <c r="K178" s="20"/>
+      <c r="L178" s="21"/>
     </row>
     <row r="179" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A179" s="11"/>
@@ -9063,8 +9179,8 @@
       <c r="H179" s="14"/>
       <c r="I179" s="14"/>
       <c r="J179" s="15"/>
-      <c r="K179" s="23"/>
-      <c r="L179" s="24"/>
+      <c r="K179" s="20"/>
+      <c r="L179" s="21"/>
     </row>
     <row r="180" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A180" s="11"/>
@@ -9077,8 +9193,8 @@
       <c r="H180" s="14"/>
       <c r="I180" s="14"/>
       <c r="J180" s="15"/>
-      <c r="K180" s="23"/>
-      <c r="L180" s="24"/>
+      <c r="K180" s="20"/>
+      <c r="L180" s="21"/>
     </row>
     <row r="181" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A181" s="11"/>
@@ -9091,8 +9207,8 @@
       <c r="H181" s="14"/>
       <c r="I181" s="14"/>
       <c r="J181" s="15"/>
-      <c r="K181" s="23"/>
-      <c r="L181" s="24"/>
+      <c r="K181" s="20"/>
+      <c r="L181" s="21"/>
     </row>
     <row r="182" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A182" s="11"/>
@@ -9105,8 +9221,8 @@
       <c r="H182" s="14"/>
       <c r="I182" s="14"/>
       <c r="J182" s="15"/>
-      <c r="K182" s="23"/>
-      <c r="L182" s="24"/>
+      <c r="K182" s="20"/>
+      <c r="L182" s="21"/>
     </row>
     <row r="183" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A183" s="11"/>
@@ -9119,8 +9235,8 @@
       <c r="H183" s="14"/>
       <c r="I183" s="14"/>
       <c r="J183" s="15"/>
-      <c r="K183" s="23"/>
-      <c r="L183" s="24"/>
+      <c r="K183" s="20"/>
+      <c r="L183" s="21"/>
     </row>
     <row r="184" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A184" s="11"/>
@@ -9133,8 +9249,8 @@
       <c r="H184" s="14"/>
       <c r="I184" s="14"/>
       <c r="J184" s="15"/>
-      <c r="K184" s="23"/>
-      <c r="L184" s="24"/>
+      <c r="K184" s="20"/>
+      <c r="L184" s="21"/>
     </row>
     <row r="185" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A185" s="11"/>
@@ -9147,8 +9263,8 @@
       <c r="H185" s="14"/>
       <c r="I185" s="14"/>
       <c r="J185" s="15"/>
-      <c r="K185" s="23"/>
-      <c r="L185" s="24"/>
+      <c r="K185" s="20"/>
+      <c r="L185" s="21"/>
     </row>
     <row r="186" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A186" s="11"/>
@@ -9161,8 +9277,8 @@
       <c r="H186" s="14"/>
       <c r="I186" s="14"/>
       <c r="J186" s="15"/>
-      <c r="K186" s="23"/>
-      <c r="L186" s="24"/>
+      <c r="K186" s="20"/>
+      <c r="L186" s="21"/>
     </row>
     <row r="187" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A187" s="11"/>
@@ -9175,8 +9291,8 @@
       <c r="H187" s="14"/>
       <c r="I187" s="14"/>
       <c r="J187" s="15"/>
-      <c r="K187" s="23"/>
-      <c r="L187" s="24"/>
+      <c r="K187" s="20"/>
+      <c r="L187" s="21"/>
     </row>
     <row r="188" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A188" s="11"/>
@@ -9189,8 +9305,8 @@
       <c r="H188" s="14"/>
       <c r="I188" s="14"/>
       <c r="J188" s="15"/>
-      <c r="K188" s="23"/>
-      <c r="L188" s="24"/>
+      <c r="K188" s="20"/>
+      <c r="L188" s="21"/>
     </row>
     <row r="189" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A189" s="11"/>
@@ -9203,8 +9319,8 @@
       <c r="H189" s="14"/>
       <c r="I189" s="14"/>
       <c r="J189" s="15"/>
-      <c r="K189" s="23"/>
-      <c r="L189" s="24"/>
+      <c r="K189" s="20"/>
+      <c r="L189" s="21"/>
     </row>
     <row r="190" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A190" s="11"/>
@@ -9217,8 +9333,8 @@
       <c r="H190" s="14"/>
       <c r="I190" s="14"/>
       <c r="J190" s="15"/>
-      <c r="K190" s="23"/>
-      <c r="L190" s="24"/>
+      <c r="K190" s="20"/>
+      <c r="L190" s="21"/>
     </row>
     <row r="191" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A191" s="11"/>
@@ -9231,8 +9347,8 @@
       <c r="H191" s="14"/>
       <c r="I191" s="14"/>
       <c r="J191" s="15"/>
-      <c r="K191" s="23"/>
-      <c r="L191" s="24"/>
+      <c r="K191" s="20"/>
+      <c r="L191" s="21"/>
     </row>
     <row r="192" s="2" customFormat="1" ht="19" customHeight="1" spans="1:12">
       <c r="A192" s="11"/>
@@ -9245,76 +9361,88 @@
       <c r="H192" s="14"/>
       <c r="I192" s="14"/>
       <c r="J192" s="15"/>
-      <c r="K192" s="23"/>
-      <c r="L192" s="24"/>
+      <c r="K192" s="20"/>
+      <c r="L192" s="21"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <conditionalFormatting sqref="N20">
-    <cfRule type="beginsWith" dxfId="0" priority="13" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="16" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N20,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="14" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N20,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="15" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N20,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23">
-    <cfRule type="beginsWith" dxfId="0" priority="7" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N23,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="8" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N23,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="9" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N23,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N24">
-    <cfRule type="beginsWith" dxfId="0" priority="16" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="19" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N24,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="17" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="20" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N24,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="18" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="21" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N24,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N33">
+    <cfRule type="beginsWith" dxfId="2" priority="3" stopIfTrue="1" operator="equal" text="PASS">
+      <formula>LEFT(N33,LEN("PASS"))="PASS"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="2" stopIfTrue="1" operator="equal" text="FAIL">
+      <formula>LEFT(N33,LEN("FAIL"))="FAIL"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="1" stopIfTrue="1" operator="equal" text="WARN">
+      <formula>LEFT(N33,LEN("WARN"))="WARN"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="N16:N19">
-    <cfRule type="beginsWith" dxfId="0" priority="22" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="25" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N16,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="23" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="26" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N16,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="24" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="27" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N16,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N21:N22">
-    <cfRule type="beginsWith" dxfId="0" priority="10" stopIfTrue="1" operator="equal" text="WARN">
+    <cfRule type="beginsWith" dxfId="0" priority="13" stopIfTrue="1" operator="equal" text="WARN">
       <formula>LEFT(N21,LEN("WARN"))="WARN"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="11" stopIfTrue="1" operator="equal" text="FAIL">
+    <cfRule type="beginsWith" dxfId="1" priority="14" stopIfTrue="1" operator="equal" text="FAIL">
       <formula>LEFT(N21,LEN("FAIL"))="FAIL"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="12" stopIfTrue="1" operator="equal" text="PASS">
+    <cfRule type="beginsWith" dxfId="2" priority="15" stopIfTrue="1" operator="equal" text="PASS">
       <formula>LEFT(N21,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D5 D6 D9 D10 D11 D12 D13 D14 D15 D18 D19 D20 D21 D22 D23 D24 D25 D2:D3 D7:D8 D16:D17 D26:D192">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4 D5 D6 D9 D10 D11 D12 D13 D14 D15 D18 D19 D20 D21 D22 D23 D24 D25 D33 D2:D3 D7:D8 D16:D17 D26:D32 D34:D192">
       <formula1>INDIRECT(C2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C11 C12 C13 C14 C15 C18 C19 C20 C21 C22 C23 C24 C25 C2:C3 C4:C5 C7:C8 C9:C10 C16:C17 C26:C192">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C11 C12 C13 C14 C15 C18 C19 C20 C21 C22 C23 C24 C25 C33 C2:C3 C4:C5 C7:C8 C9:C10 C16:C17 C26:C32 C34:C192">
       <formula1>target</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E16" r:id="rId1" display="${uiurl}" tooltip="https://gnukhata.gitlab.io/gkapp/#/user-login"/>
+    <hyperlink ref="E25" r:id="rId1" display="${uiurl}" tooltip="https://gnukhata.gitlab.io/gkapp/#/user-login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
UI Manage Users script
</commit_message>
<xml_diff>
--- a/tests/artifact/script/GNUKhata.macro.xlsx
+++ b/tests/artifact/script/GNUKhata.macro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="782">
   <si>
     <t>target</t>
   </si>
@@ -2479,16 +2479,19 @@
   <si>
     <t>${title.header}</t>
   </si>
+  <si>
+    <t>Welcome Accion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -2540,21 +2543,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -2563,18 +2551,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2587,6 +2591,37 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2594,15 +2629,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2616,55 +2652,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2679,6 +2668,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2705,7 +2708,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2717,7 +2720,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2729,7 +2738,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2741,19 +2846,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2765,127 +2888,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2915,16 +2918,34 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2944,37 +2965,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3005,16 +3006,24 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3023,139 +3032,133 @@
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3223,7 +3226,7 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -3250,52 +3253,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -3617,7 +3620,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="18" width="8.33333333333333" customWidth="1" collapsed="1"/>
   </cols>
@@ -6287,13 +6290,13 @@
   <sheetPr/>
   <dimension ref="A1:O192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="$A24:$XFD24"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20.1666666666667" style="3" customWidth="1"/>
     <col min="2" max="2" width="31.5" style="4" customWidth="1"/>
@@ -6345,7 +6348,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="41.4" spans="1:12">
+    <row r="2" s="2" customFormat="1" ht="42" spans="1:12">
       <c r="A2" s="11" t="s">
         <v>734</v>
       </c>
@@ -6439,7 +6442,7 @@
       <c r="K5" s="23"/>
       <c r="L5" s="24"/>
     </row>
-    <row r="6" s="2" customFormat="1" ht="41.4" spans="1:12">
+    <row r="6" s="2" customFormat="1" ht="42" spans="1:12">
       <c r="A6" s="11" t="s">
         <v>744</v>
       </c>
@@ -6553,7 +6556,7 @@
       <c r="K10" s="23"/>
       <c r="L10" s="24"/>
     </row>
-    <row r="11" s="2" customFormat="1" ht="96.6" spans="1:12">
+    <row r="11" s="2" customFormat="1" ht="98" spans="1:12">
       <c r="A11" s="11" t="s">
         <v>750</v>
       </c>
@@ -6667,7 +6670,7 @@
       <c r="K15" s="23"/>
       <c r="L15" s="24"/>
     </row>
-    <row r="16" s="2" customFormat="1" ht="27.6" spans="1:15">
+    <row r="16" s="2" customFormat="1" ht="28" spans="1:15">
       <c r="A16" s="11" t="s">
         <v>762</v>
       </c>
@@ -6880,12 +6883,14 @@
         <v>30</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>559</v>
+        <v>535</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>780</v>
       </c>
-      <c r="F24" s="15"/>
+      <c r="F24" s="15" t="s">
+        <v>781</v>
+      </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>

</xml_diff>

<commit_message>
Changes in UI-StockOnHand script
</commit_message>
<xml_diff>
--- a/tests/artifact/script/GNUKhata.macro.xlsx
+++ b/tests/artifact/script/GNUKhata.macro.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="18350" windowHeight="6920" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="#system" sheetId="4" state="hidden" r:id="rId1"/>
@@ -56,7 +56,20 @@
     <definedName name="javaui">'#system'!$N$2:$N$16</definedName>
     <definedName name="browserstack">'#system'!$G$2:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2495,7 +2508,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -6291,7 +6304,7 @@
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333333333333" defaultRowHeight="14.5"/>

</xml_diff>